<commit_message>
Implement ThSprinklerRoomChecker & Update ThMEPEngineCoreRoomService as base class (#825)
Co-authored-by: 刘潘 <liupan1@thape.com.cn>
</commit_message>
<xml_diff>
--- a/AutoLoader/Contents/Support/房间名称分类处理.xlsx
+++ b/AutoLoader/Contents/Support/房间名称分类处理.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\Autodesk\ApplicationPlugins\ThMEPPlugin.bundle\Contents\Support\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12540"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="房间名称处理" sheetId="1" r:id="rId1"/>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="462">
   <si>
     <t>一级</t>
   </si>
@@ -1333,62 +1338,89 @@
     <t>无燃气餐饮</t>
   </si>
   <si>
+    <t>零售</t>
+  </si>
+  <si>
+    <t>超市</t>
+  </si>
+  <si>
+    <t>私有区域；感烟火灾探测器；疏散指示；疏散照明</t>
+  </si>
+  <si>
+    <t>营业厅</t>
+  </si>
+  <si>
+    <t>观演建筑</t>
+  </si>
+  <si>
+    <t>电影院</t>
+  </si>
+  <si>
+    <t>观众厅</t>
+  </si>
+  <si>
+    <t>观众休息厅</t>
+  </si>
+  <si>
+    <t>放映设备间</t>
+  </si>
+  <si>
+    <t>剧院</t>
+  </si>
+  <si>
+    <t>剧场</t>
+  </si>
+  <si>
+    <t>音乐厅</t>
+  </si>
+  <si>
+    <t>排演厅</t>
+  </si>
+  <si>
+    <t>化妆室</t>
+  </si>
+  <si>
+    <t>其他空间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>电餐</t>
-  </si>
-  <si>
-    <t>零售</t>
-  </si>
-  <si>
-    <t>超市</t>
-  </si>
-  <si>
-    <t>私有区域；感烟火灾探测器；疏散指示；疏散照明</t>
-  </si>
-  <si>
-    <t>营业厅</t>
-  </si>
-  <si>
-    <t>观演建筑</t>
-  </si>
-  <si>
-    <t>电影院</t>
-  </si>
-  <si>
-    <t>观众厅</t>
-  </si>
-  <si>
-    <t>观众休息厅</t>
-  </si>
-  <si>
-    <t>放映设备间</t>
-  </si>
-  <si>
-    <t>剧院</t>
-  </si>
-  <si>
-    <t>剧场</t>
-  </si>
-  <si>
-    <t>音乐厅</t>
-  </si>
-  <si>
-    <t>排演厅</t>
-  </si>
-  <si>
-    <t>化妆室</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>游泳池</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>溜冰场</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>滑雪场</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>溜冰、冰场</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>滑雪、雪场</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>游泳、泳池</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>地库配电间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="21">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1397,169 +1429,26 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <sz val="9"/>
       <name val="等线"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="35">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1569,192 +1458,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -1762,253 +1471,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2019,70 +1486,38 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="00336699"/>
+      <color rgb="FF336699"/>
     </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2340,37 +1775,37 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:F295"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F298"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="20.625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="23.5" style="4" customWidth="1"/>
     <col min="4" max="4" width="20.625" style="1" customWidth="1"/>
     <col min="5" max="5" width="50.625" style="2" customWidth="1"/>
     <col min="6" max="6" width="66.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -2383,13 +1818,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:6">
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -2397,8 +1832,8 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="3:6">
-      <c r="C4" s="1" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C4" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -2411,8 +1846,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="3:6">
-      <c r="C5" s="1" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C5" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -2422,15 +1857,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="3:6">
-      <c r="C6" s="1" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C6" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="4:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D7" s="1" t="s">
         <v>17</v>
       </c>
@@ -2438,7 +1873,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="4:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D8" s="1" t="s">
         <v>19</v>
       </c>
@@ -2446,7 +1881,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="4:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D9" s="1" t="s">
         <v>20</v>
       </c>
@@ -2457,8 +1892,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="3:6">
-      <c r="C10" s="1" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C10" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -2471,8 +1906,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="3:6">
-      <c r="C11" s="1" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C11" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -2485,40 +1920,40 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="3:6">
-      <c r="C12" s="1" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C12" s="4" t="s">
         <v>27</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="3:6">
-      <c r="C13" s="1" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C13" s="4" t="s">
         <v>28</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="3:6">
-      <c r="C14" s="1" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C14" s="4" t="s">
         <v>29</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="3:6">
-      <c r="C15" s="1" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C15" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="3:6">
-      <c r="C16" s="2" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C16" s="5" t="s">
         <v>31</v>
       </c>
       <c r="E16" s="2" t="s">
@@ -2528,8 +1963,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="3:6">
-      <c r="C17" s="1" t="s">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C17" s="4" t="s">
         <v>33</v>
       </c>
       <c r="E17" s="2" t="s">
@@ -2539,8 +1974,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="3:6">
-      <c r="C18" s="1" t="s">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C18" s="4" t="s">
         <v>35</v>
       </c>
       <c r="E18" s="2" t="s">
@@ -2550,7 +1985,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="4:6">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D19" s="1" t="s">
         <v>37</v>
       </c>
@@ -2558,7 +1993,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="4:6">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D20" s="1" t="s">
         <v>38</v>
       </c>
@@ -2566,16 +2001,16 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="3:6">
-      <c r="C21" s="1" t="s">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C21" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="3:6">
-      <c r="C22" s="1" t="s">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C22" s="4" t="s">
         <v>40</v>
       </c>
       <c r="E22" s="2" t="s">
@@ -2585,8 +2020,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="3:6">
-      <c r="C23" s="1" t="s">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C23" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E23" s="2" t="s">
@@ -2596,16 +2031,16 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="2:6">
-      <c r="B24" s="1" t="s">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B24" s="4" t="s">
         <v>45</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="3:6">
-      <c r="C25" s="3" t="s">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C25" s="4" t="s">
         <v>47</v>
       </c>
       <c r="E25" s="2" t="s">
@@ -2615,7 +2050,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="4:6">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D26" s="1" t="s">
         <v>50</v>
       </c>
@@ -2623,7 +2058,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="4:6">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D27" s="1" t="s">
         <v>52</v>
       </c>
@@ -2634,7 +2069,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="4:6">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D28" s="1" t="s">
         <v>54</v>
       </c>
@@ -2645,7 +2080,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="4:6">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D29" s="1" t="s">
         <v>56</v>
       </c>
@@ -2653,8 +2088,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="3:6">
-      <c r="C30" s="3" t="s">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C30" s="4" t="s">
         <v>57</v>
       </c>
       <c r="E30" s="2" t="s">
@@ -2664,7 +2099,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="4:6">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D31" s="1" t="s">
         <v>60</v>
       </c>
@@ -2675,7 +2110,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="4:6">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D32" s="1" t="s">
         <v>62</v>
       </c>
@@ -2686,7 +2121,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="4:6">
+    <row r="33" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D33" s="1" t="s">
         <v>64</v>
       </c>
@@ -2697,7 +2132,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="4:6">
+    <row r="34" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D34" s="1" t="s">
         <v>67</v>
       </c>
@@ -2708,7 +2143,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="4:6">
+    <row r="35" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D35" s="1" t="s">
         <v>69</v>
       </c>
@@ -2719,8 +2154,8 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="3:6">
-      <c r="C36" s="1" t="s">
+    <row r="36" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C36" s="4" t="s">
         <v>71</v>
       </c>
       <c r="E36" s="2" t="s">
@@ -2730,7 +2165,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="4:6">
+    <row r="37" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D37" s="1" t="s">
         <v>73</v>
       </c>
@@ -2738,7 +2173,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="38" spans="4:6">
+    <row r="38" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D38" s="1" t="s">
         <v>74</v>
       </c>
@@ -2749,15 +2184,15 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="3:6">
-      <c r="C39" s="1" t="s">
+    <row r="39" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C39" s="4" t="s">
         <v>76</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="4:6">
+    <row r="40" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D40" s="1" t="s">
         <v>77</v>
       </c>
@@ -2765,7 +2200,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="41" spans="4:6">
+    <row r="41" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D41" s="1" t="s">
         <v>78</v>
       </c>
@@ -2773,24 +2208,24 @@
         <v>66</v>
       </c>
     </row>
-    <row r="42" spans="3:6">
-      <c r="C42" s="1" t="s">
+    <row r="42" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C42" s="4" t="s">
         <v>79</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="43" spans="3:6">
-      <c r="C43" s="1" t="s">
+    <row r="43" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C43" s="4" t="s">
         <v>81</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="44" spans="3:6">
-      <c r="C44" s="1" t="s">
+    <row r="44" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C44" s="4" t="s">
         <v>82</v>
       </c>
       <c r="E44" s="2" t="s">
@@ -2800,16 +2235,16 @@
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="3:6">
-      <c r="C45" s="1" t="s">
+    <row r="45" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C45" s="4" t="s">
         <v>84</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="46" spans="3:6">
-      <c r="C46" s="1" t="s">
+    <row r="46" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C46" s="4" t="s">
         <v>85</v>
       </c>
       <c r="E46" s="2" t="s">
@@ -2819,8 +2254,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="47" spans="3:6">
-      <c r="C47" s="1" t="s">
+    <row r="47" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C47" s="4" t="s">
         <v>87</v>
       </c>
       <c r="E47" s="2" t="s">
@@ -2830,16 +2265,16 @@
         <v>51</v>
       </c>
     </row>
-    <row r="48" spans="3:6">
-      <c r="C48" s="1" t="s">
+    <row r="48" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C48" s="4" t="s">
         <v>89</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="49" spans="3:6">
-      <c r="C49" s="1" t="s">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C49" s="4" t="s">
         <v>90</v>
       </c>
       <c r="E49" s="2" t="s">
@@ -2849,7 +2284,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="4:6">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D50" s="1" t="s">
         <v>92</v>
       </c>
@@ -2860,7 +2295,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="4:6">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D51" s="1" t="s">
         <v>94</v>
       </c>
@@ -2871,7 +2306,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="4:6">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D52" s="1" t="s">
         <v>96</v>
       </c>
@@ -2879,7 +2314,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="53" spans="4:6">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D53" s="1" t="s">
         <v>97</v>
       </c>
@@ -2890,16 +2325,16 @@
         <v>80</v>
       </c>
     </row>
-    <row r="54" spans="2:6">
-      <c r="B54" s="4" t="s">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B54" s="3" t="s">
         <v>99</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="55" spans="3:6">
-      <c r="C55" s="1" t="s">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C55" s="4" t="s">
         <v>101</v>
       </c>
       <c r="E55" s="2" t="s">
@@ -2909,7 +2344,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="56" spans="4:6">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D56" s="1" t="s">
         <v>104</v>
       </c>
@@ -2920,7 +2355,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="57" spans="4:6">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D57" s="1" t="s">
         <v>106</v>
       </c>
@@ -2931,7 +2366,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="58" spans="4:6">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D58" s="1" t="s">
         <v>108</v>
       </c>
@@ -2942,7 +2377,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="59" spans="4:6">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D59" s="1" t="s">
         <v>110</v>
       </c>
@@ -2953,7 +2388,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="60" spans="4:6">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D60" s="1" t="s">
         <v>112</v>
       </c>
@@ -2961,7 +2396,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="61" spans="4:6">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D61" s="1" t="s">
         <v>113</v>
       </c>
@@ -2969,7 +2404,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="62" spans="4:6">
+    <row r="62" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D62" s="1" t="s">
         <v>114</v>
       </c>
@@ -2977,7 +2412,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="63" spans="4:6">
+    <row r="63" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D63" s="1" t="s">
         <v>115</v>
       </c>
@@ -2985,7 +2420,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="64" spans="4:6">
+    <row r="64" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D64" s="1" t="s">
         <v>116</v>
       </c>
@@ -2993,7 +2428,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="65" spans="4:6">
+    <row r="65" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D65" s="1" t="s">
         <v>117</v>
       </c>
@@ -3001,7 +2436,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="66" spans="4:6">
+    <row r="66" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D66" s="1" t="s">
         <v>118</v>
       </c>
@@ -3012,7 +2447,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="67" spans="4:6">
+    <row r="67" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D67" s="1" t="s">
         <v>120</v>
       </c>
@@ -3023,8 +2458,8 @@
         <v>103</v>
       </c>
     </row>
-    <row r="68" spans="3:6">
-      <c r="C68" s="1" t="s">
+    <row r="68" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C68" s="4" t="s">
         <v>122</v>
       </c>
       <c r="E68" s="2" t="s">
@@ -3034,8 +2469,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="69" spans="3:6">
-      <c r="C69" s="1" t="s">
+    <row r="69" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C69" s="4" t="s">
         <v>124</v>
       </c>
       <c r="E69" s="2" t="s">
@@ -3045,16 +2480,16 @@
         <v>16</v>
       </c>
     </row>
-    <row r="70" spans="3:6">
-      <c r="C70" s="1" t="s">
+    <row r="70" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C70" s="4" t="s">
         <v>126</v>
       </c>
       <c r="F70" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="71" spans="4:6">
-      <c r="D71" s="1" t="s">
+    <row r="71" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D71" s="6" t="s">
         <v>127</v>
       </c>
       <c r="E71" s="2" t="s">
@@ -3064,7 +2499,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="72" spans="4:6">
+    <row r="72" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D72" s="1" t="s">
         <v>130</v>
       </c>
@@ -3075,7 +2510,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="73" ht="28.5" spans="4:6">
+    <row r="73" spans="2:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="D73" s="1" t="s">
         <v>133</v>
       </c>
@@ -3086,7 +2521,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="74" spans="4:6">
+    <row r="74" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D74" s="1" t="s">
         <v>135</v>
       </c>
@@ -3097,7 +2532,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="75" spans="4:6">
+    <row r="75" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D75" s="1" t="s">
         <v>138</v>
       </c>
@@ -3108,8 +2543,8 @@
         <v>137</v>
       </c>
     </row>
-    <row r="76" spans="3:6">
-      <c r="C76" s="1" t="s">
+    <row r="76" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C76" s="4" t="s">
         <v>140</v>
       </c>
       <c r="E76" s="2" t="s">
@@ -3119,7 +2554,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="77" spans="4:6">
+    <row r="77" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D77" s="1" t="s">
         <v>142</v>
       </c>
@@ -3130,7 +2565,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="78" spans="4:6">
+    <row r="78" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D78" s="1" t="s">
         <v>144</v>
       </c>
@@ -3141,7 +2576,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="79" ht="28.5" spans="4:6">
+    <row r="79" spans="2:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="D79" s="1" t="s">
         <v>146</v>
       </c>
@@ -3152,7 +2587,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="80" spans="2:6">
+    <row r="80" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B80" s="4" t="s">
         <v>148</v>
       </c>
@@ -3163,8 +2598,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="81" spans="3:6">
-      <c r="C81" s="1" t="s">
+    <row r="81" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C81" s="4" t="s">
         <v>150</v>
       </c>
       <c r="E81" s="2" t="s">
@@ -3174,7 +2609,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="82" spans="4:6">
+    <row r="82" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D82" s="1" t="s">
         <v>153</v>
       </c>
@@ -3182,7 +2617,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="83" spans="4:6">
+    <row r="83" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D83" s="1" t="s">
         <v>154</v>
       </c>
@@ -3193,7 +2628,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="84" spans="4:6">
+    <row r="84" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D84" s="1" t="s">
         <v>156</v>
       </c>
@@ -3201,7 +2636,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="85" spans="4:6">
+    <row r="85" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D85" s="1" t="s">
         <v>157</v>
       </c>
@@ -3209,15 +2644,15 @@
         <v>152</v>
       </c>
     </row>
-    <row r="86" spans="3:6">
-      <c r="C86" s="1" t="s">
+    <row r="86" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C86" s="4" t="s">
         <v>158</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="87" spans="4:6">
+    <row r="87" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D87" s="1" t="s">
         <v>160</v>
       </c>
@@ -3225,8 +2660,8 @@
         <v>159</v>
       </c>
     </row>
-    <row r="88" spans="3:6">
-      <c r="C88" s="1" t="s">
+    <row r="88" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C88" s="4" t="s">
         <v>161</v>
       </c>
       <c r="E88" s="2" t="s">
@@ -3236,8 +2671,8 @@
         <v>159</v>
       </c>
     </row>
-    <row r="89" spans="3:6">
-      <c r="C89" s="1" t="s">
+    <row r="89" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C89" s="4" t="s">
         <v>163</v>
       </c>
       <c r="E89" s="2" t="s">
@@ -3247,8 +2682,8 @@
         <v>152</v>
       </c>
     </row>
-    <row r="90" spans="3:6">
-      <c r="C90" s="1" t="s">
+    <row r="90" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C90" s="4" t="s">
         <v>165</v>
       </c>
       <c r="E90" s="2" t="s">
@@ -3258,7 +2693,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="91" spans="4:6">
+    <row r="91" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D91" s="1" t="s">
         <v>167</v>
       </c>
@@ -3266,64 +2701,64 @@
         <v>152</v>
       </c>
     </row>
-    <row r="92" spans="3:6">
-      <c r="C92" s="1" t="s">
+    <row r="92" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C92" s="4" t="s">
         <v>168</v>
       </c>
       <c r="F92" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="93" spans="3:6">
-      <c r="C93" s="1" t="s">
+    <row r="93" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C93" s="4" t="s">
         <v>169</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="94" spans="3:6">
-      <c r="C94" s="1" t="s">
+    <row r="94" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C94" s="4" t="s">
         <v>170</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="95" spans="3:6">
-      <c r="C95" s="1" t="s">
+    <row r="95" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C95" s="4" t="s">
         <v>171</v>
       </c>
       <c r="F95" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="96" spans="3:6">
-      <c r="C96" s="1" t="s">
+    <row r="96" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C96" s="4" t="s">
         <v>172</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="97" spans="3:6">
-      <c r="C97" s="1" t="s">
+    <row r="97" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C97" s="4" t="s">
         <v>173</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="98" spans="3:6">
-      <c r="C98" s="1" t="s">
+    <row r="98" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C98" s="4" t="s">
         <v>174</v>
       </c>
       <c r="F98" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="99" spans="3:6">
-      <c r="C99" s="1" t="s">
+    <row r="99" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C99" s="4" t="s">
         <v>175</v>
       </c>
       <c r="E99" s="2" t="s">
@@ -3333,8 +2768,8 @@
         <v>152</v>
       </c>
     </row>
-    <row r="100" spans="3:6">
-      <c r="C100" s="1" t="s">
+    <row r="100" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C100" s="4" t="s">
         <v>177</v>
       </c>
       <c r="E100" s="2" t="s">
@@ -3344,7 +2779,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="101" spans="4:6">
+    <row r="101" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D101" s="1" t="s">
         <v>179</v>
       </c>
@@ -3352,8 +2787,8 @@
         <v>152</v>
       </c>
     </row>
-    <row r="102" spans="3:6">
-      <c r="C102" s="1" t="s">
+    <row r="102" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C102" s="4" t="s">
         <v>180</v>
       </c>
       <c r="E102" s="2" t="s">
@@ -3363,7 +2798,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="103" spans="4:6">
+    <row r="103" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D103" s="1" t="s">
         <v>182</v>
       </c>
@@ -3371,7 +2806,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="104" spans="4:6">
+    <row r="104" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D104" s="1" t="s">
         <v>183</v>
       </c>
@@ -3379,15 +2814,15 @@
         <v>159</v>
       </c>
     </row>
-    <row r="105" spans="3:6">
-      <c r="C105" s="1" t="s">
+    <row r="105" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C105" s="4" t="s">
         <v>184</v>
       </c>
       <c r="F105" s="1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="106" spans="4:6">
+    <row r="106" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D106" s="1" t="s">
         <v>186</v>
       </c>
@@ -3395,7 +2830,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="107" spans="4:6">
+    <row r="107" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D107" s="1" t="s">
         <v>187</v>
       </c>
@@ -3403,7 +2838,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="108" spans="4:6">
+    <row r="108" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D108" s="1" t="s">
         <v>188</v>
       </c>
@@ -3411,7 +2846,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="109" spans="4:6">
+    <row r="109" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D109" s="1" t="s">
         <v>189</v>
       </c>
@@ -3419,87 +2854,87 @@
         <v>16</v>
       </c>
     </row>
-    <row r="110" spans="2:6">
-      <c r="B110" s="1" t="s">
+    <row r="110" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B110" s="4" t="s">
         <v>190</v>
       </c>
       <c r="F110" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="111" spans="3:6">
-      <c r="C111" s="1" t="s">
+    <row r="111" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C111" s="4" t="s">
         <v>191</v>
       </c>
       <c r="F111" s="1" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="112" spans="3:6">
-      <c r="C112" s="1" t="s">
+    <row r="112" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C112" s="4" t="s">
         <v>193</v>
       </c>
       <c r="F112" s="1" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="113" spans="3:6">
-      <c r="C113" s="1" t="s">
+    <row r="113" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C113" s="4" t="s">
         <v>194</v>
       </c>
       <c r="F113" s="1" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="114" spans="2:6">
-      <c r="B114" s="1" t="s">
+    <row r="114" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B114" s="4" t="s">
         <v>195</v>
       </c>
       <c r="F114" s="1" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="115" spans="3:6">
-      <c r="C115" s="1" t="s">
+    <row r="115" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C115" s="4" t="s">
         <v>196</v>
       </c>
       <c r="F115" s="1" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="116" spans="3:6">
-      <c r="C116" s="1" t="s">
+    <row r="116" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C116" s="4" t="s">
         <v>197</v>
       </c>
       <c r="F116" s="1" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="117" spans="2:6">
-      <c r="B117" s="1" t="s">
+    <row r="117" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B117" s="3" t="s">
         <v>198</v>
       </c>
       <c r="F117" s="1" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="118" spans="3:6">
-      <c r="C118" s="1" t="s">
+    <row r="118" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C118" s="4" t="s">
         <v>199</v>
       </c>
       <c r="F118" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="119" spans="3:6">
-      <c r="C119" s="1" t="s">
+    <row r="119" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C119" s="4" t="s">
         <v>200</v>
       </c>
       <c r="F119" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="120" ht="57" spans="4:6">
+    <row r="120" spans="2:6" ht="57" x14ac:dyDescent="0.2">
       <c r="D120" s="1" t="s">
         <v>201</v>
       </c>
@@ -3510,16 +2945,16 @@
         <v>203</v>
       </c>
     </row>
-    <row r="121" spans="3:6">
-      <c r="C121" s="1" t="s">
+    <row r="121" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C121" s="4" t="s">
         <v>204</v>
       </c>
       <c r="F121" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="122" spans="3:6">
-      <c r="C122" s="1" t="s">
+    <row r="122" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C122" s="4" t="s">
         <v>205</v>
       </c>
       <c r="E122" s="2" t="s">
@@ -3529,8 +2964,8 @@
         <v>203</v>
       </c>
     </row>
-    <row r="123" ht="57" spans="3:6">
-      <c r="C123" s="1" t="s">
+    <row r="123" spans="2:6" ht="57" x14ac:dyDescent="0.2">
+      <c r="C123" s="4" t="s">
         <v>207</v>
       </c>
       <c r="E123" s="2" t="s">
@@ -3540,8 +2975,8 @@
         <v>203</v>
       </c>
     </row>
-    <row r="124" spans="3:6">
-      <c r="C124" s="1" t="s">
+    <row r="124" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C124" s="4" t="s">
         <v>209</v>
       </c>
       <c r="E124" s="2" t="s">
@@ -3551,15 +2986,15 @@
         <v>203</v>
       </c>
     </row>
-    <row r="125" spans="3:6">
-      <c r="C125" s="1" t="s">
+    <row r="125" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C125" s="4" t="s">
         <v>211</v>
       </c>
       <c r="F125" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="126" spans="4:6">
+    <row r="126" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D126" s="1" t="s">
         <v>212</v>
       </c>
@@ -3570,7 +3005,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="127" spans="4:6">
+    <row r="127" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D127" s="1" t="s">
         <v>214</v>
       </c>
@@ -3581,7 +3016,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="128" spans="4:6">
+    <row r="128" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D128" s="1" t="s">
         <v>216</v>
       </c>
@@ -3592,7 +3027,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="129" ht="28.5" spans="1:6">
+    <row r="129" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A129" s="4" t="s">
         <v>218</v>
       </c>
@@ -3603,31 +3038,34 @@
         <v>220</v>
       </c>
     </row>
-    <row r="130" spans="2:6">
-      <c r="B130" s="1" t="s">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B130" s="3" t="s">
         <v>221</v>
       </c>
       <c r="F130" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="131" spans="3:6">
-      <c r="C131" s="1" t="s">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C131" s="4" t="s">
         <v>222</v>
+      </c>
+      <c r="E131" s="2" t="s">
+        <v>461</v>
       </c>
       <c r="F131" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="132" spans="3:6">
-      <c r="C132" s="1" t="s">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C132" s="4" t="s">
         <v>223</v>
       </c>
       <c r="F132" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="133" spans="4:6">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D133" s="1" t="s">
         <v>224</v>
       </c>
@@ -3638,7 +3076,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="134" spans="4:6">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D134" s="1" t="s">
         <v>226</v>
       </c>
@@ -3649,8 +3087,8 @@
         <v>203</v>
       </c>
     </row>
-    <row r="135" spans="3:6">
-      <c r="C135" s="1" t="s">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C135" s="4" t="s">
         <v>228</v>
       </c>
       <c r="E135" s="2" t="s">
@@ -3660,7 +3098,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="136" spans="4:6">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D136" s="1" t="s">
         <v>230</v>
       </c>
@@ -3668,15 +3106,15 @@
         <v>203</v>
       </c>
     </row>
-    <row r="137" spans="3:6">
-      <c r="C137" s="1" t="s">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C137" s="4" t="s">
         <v>231</v>
       </c>
       <c r="F137" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="138" spans="4:6">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D138" s="1" t="s">
         <v>232</v>
       </c>
@@ -3687,8 +3125,8 @@
         <v>203</v>
       </c>
     </row>
-    <row r="139" ht="42.75" spans="3:6">
-      <c r="C139" s="1" t="s">
+    <row r="139" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="C139" s="4" t="s">
         <v>234</v>
       </c>
       <c r="E139" s="2" t="s">
@@ -3698,24 +3136,24 @@
         <v>203</v>
       </c>
     </row>
-    <row r="140" spans="3:6">
-      <c r="C140" s="1" t="s">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C140" s="4" t="s">
         <v>236</v>
       </c>
       <c r="F140" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="141" spans="3:6">
-      <c r="C141" s="1" t="s">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C141" s="4" t="s">
         <v>237</v>
       </c>
       <c r="F141" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="142" spans="2:6">
-      <c r="B142" s="1" t="s">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B142" s="3" t="s">
         <v>238</v>
       </c>
       <c r="E142" s="2" t="s">
@@ -3725,8 +3163,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="143" spans="3:6">
-      <c r="C143" s="1" t="s">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C143" s="4" t="s">
         <v>240</v>
       </c>
       <c r="E143" s="2" t="s">
@@ -3736,16 +3174,16 @@
         <v>152</v>
       </c>
     </row>
-    <row r="144" spans="3:6">
-      <c r="C144" s="1" t="s">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C144" s="4" t="s">
         <v>242</v>
       </c>
       <c r="F144" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="145" spans="3:6">
-      <c r="C145" s="1" t="s">
+    <row r="145" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C145" s="4" t="s">
         <v>243</v>
       </c>
       <c r="E145" s="2" t="s">
@@ -3755,8 +3193,8 @@
         <v>152</v>
       </c>
     </row>
-    <row r="146" ht="28.5" spans="3:6">
-      <c r="C146" s="1" t="s">
+    <row r="146" spans="2:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="C146" s="4" t="s">
         <v>245</v>
       </c>
       <c r="E146" s="2" t="s">
@@ -3766,16 +3204,16 @@
         <v>152</v>
       </c>
     </row>
-    <row r="147" spans="3:6">
-      <c r="C147" s="1" t="s">
+    <row r="147" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C147" s="4" t="s">
         <v>247</v>
       </c>
       <c r="F147" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="148" spans="3:6">
-      <c r="C148" s="1" t="s">
+    <row r="148" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C148" s="4" t="s">
         <v>248</v>
       </c>
       <c r="E148" s="2" t="s">
@@ -3785,32 +3223,32 @@
         <v>152</v>
       </c>
     </row>
-    <row r="149" spans="2:6">
-      <c r="B149" s="1" t="s">
+    <row r="149" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B149" s="4" t="s">
         <v>250</v>
       </c>
       <c r="F149" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="150" spans="2:6">
-      <c r="B150" s="1" t="s">
+    <row r="150" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B150" s="4" t="s">
         <v>251</v>
       </c>
       <c r="F150" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="151" spans="2:6">
-      <c r="B151" s="1" t="s">
+    <row r="151" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B151" s="4" t="s">
         <v>252</v>
       </c>
       <c r="F151" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="152" spans="2:6">
-      <c r="B152" s="1" t="s">
+    <row r="152" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B152" s="4" t="s">
         <v>253</v>
       </c>
       <c r="E152" s="2" t="s">
@@ -3820,16 +3258,16 @@
         <v>152</v>
       </c>
     </row>
-    <row r="153" spans="2:6">
-      <c r="B153" s="1" t="s">
+    <row r="153" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B153" s="4" t="s">
         <v>255</v>
       </c>
       <c r="F153" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="154" spans="3:6">
-      <c r="C154" s="1" t="s">
+    <row r="154" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C154" s="4" t="s">
         <v>256</v>
       </c>
       <c r="E154" s="2" t="s">
@@ -3839,7 +3277,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="155" spans="4:6">
+    <row r="155" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D155" s="1" t="s">
         <v>258</v>
       </c>
@@ -3850,7 +3288,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="156" spans="4:6">
+    <row r="156" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D156" s="1" t="s">
         <v>260</v>
       </c>
@@ -3861,7 +3299,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="157" spans="4:6">
+    <row r="157" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D157" s="1" t="s">
         <v>262</v>
       </c>
@@ -3869,7 +3307,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="158" spans="4:6">
+    <row r="158" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D158" s="1" t="s">
         <v>263</v>
       </c>
@@ -3877,7 +3315,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="159" spans="4:6">
+    <row r="159" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D159" s="1" t="s">
         <v>264</v>
       </c>
@@ -3885,15 +3323,15 @@
         <v>152</v>
       </c>
     </row>
-    <row r="160" spans="3:6">
-      <c r="C160" s="1" t="s">
+    <row r="160" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C160" s="4" t="s">
         <v>265</v>
       </c>
       <c r="F160" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="161" spans="4:6">
+    <row r="161" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D161" s="1" t="s">
         <v>266</v>
       </c>
@@ -3901,7 +3339,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="162" spans="4:6">
+    <row r="162" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D162" s="1" t="s">
         <v>267</v>
       </c>
@@ -3909,7 +3347,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="163" spans="4:6">
+    <row r="163" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D163" s="1" t="s">
         <v>268</v>
       </c>
@@ -3917,7 +3355,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="164" spans="4:6">
+    <row r="164" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D164" s="1" t="s">
         <v>269</v>
       </c>
@@ -3925,8 +3363,8 @@
         <v>152</v>
       </c>
     </row>
-    <row r="165" spans="3:6">
-      <c r="C165" s="1" t="s">
+    <row r="165" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C165" s="4" t="s">
         <v>270</v>
       </c>
       <c r="E165" s="2" t="s">
@@ -3936,8 +3374,8 @@
         <v>152</v>
       </c>
     </row>
-    <row r="166" spans="3:6">
-      <c r="C166" s="1" t="s">
+    <row r="166" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C166" s="4" t="s">
         <v>272</v>
       </c>
       <c r="E166" s="2" t="s">
@@ -3947,8 +3385,8 @@
         <v>152</v>
       </c>
     </row>
-    <row r="167" spans="3:6">
-      <c r="C167" s="1" t="s">
+    <row r="167" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C167" s="4" t="s">
         <v>274</v>
       </c>
       <c r="E167" s="2" t="s">
@@ -3958,71 +3396,71 @@
         <v>152</v>
       </c>
     </row>
-    <row r="168" spans="2:6">
-      <c r="B168" s="1" t="s">
+    <row r="168" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B168" s="4" t="s">
         <v>276</v>
       </c>
       <c r="F168" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="169" spans="3:6">
-      <c r="C169" s="1" t="s">
+    <row r="169" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C169" s="4" t="s">
         <v>277</v>
       </c>
       <c r="F169" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="170" spans="3:6">
-      <c r="C170" s="1" t="s">
+    <row r="170" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C170" s="4" t="s">
         <v>278</v>
       </c>
       <c r="F170" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="171" spans="3:6">
-      <c r="C171" s="1" t="s">
+    <row r="171" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C171" s="4" t="s">
         <v>279</v>
       </c>
       <c r="F171" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="172" spans="3:6">
-      <c r="C172" s="1" t="s">
+    <row r="172" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C172" s="4" t="s">
         <v>280</v>
       </c>
       <c r="F172" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="173" spans="3:6">
-      <c r="C173" s="1" t="s">
+    <row r="173" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C173" s="4" t="s">
         <v>281</v>
       </c>
       <c r="F173" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="174" spans="3:6">
-      <c r="C174" s="1" t="s">
+    <row r="174" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C174" s="4" t="s">
         <v>282</v>
       </c>
       <c r="F174" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="175" spans="3:6">
-      <c r="C175" s="1" t="s">
+    <row r="175" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C175" s="4" t="s">
         <v>283</v>
       </c>
       <c r="F175" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="176" spans="4:6">
+    <row r="176" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D176" s="1" t="s">
         <v>284</v>
       </c>
@@ -4030,7 +3468,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="177" spans="4:6">
+    <row r="177" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D177" s="1" t="s">
         <v>285</v>
       </c>
@@ -4038,7 +3476,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="178" spans="4:6">
+    <row r="178" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D178" s="1" t="s">
         <v>286</v>
       </c>
@@ -4046,15 +3484,15 @@
         <v>152</v>
       </c>
     </row>
-    <row r="179" spans="3:6">
-      <c r="C179" s="1" t="s">
+    <row r="179" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C179" s="4" t="s">
         <v>287</v>
       </c>
       <c r="F179" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="180" spans="4:6">
+    <row r="180" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D180" s="1" t="s">
         <v>288</v>
       </c>
@@ -4062,32 +3500,32 @@
         <v>152</v>
       </c>
     </row>
-    <row r="181" spans="2:6">
-      <c r="B181" s="1" t="s">
+    <row r="181" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B181" s="4" t="s">
         <v>289</v>
       </c>
       <c r="F181" s="1" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="182" spans="3:6">
-      <c r="C182" s="1" t="s">
+    <row r="182" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C182" s="4" t="s">
         <v>291</v>
       </c>
       <c r="F182" s="1" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="183" spans="3:6">
-      <c r="C183" s="1" t="s">
+    <row r="183" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C183" s="4" t="s">
         <v>293</v>
       </c>
       <c r="F183" s="1" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="184" spans="3:6">
-      <c r="C184" s="1" t="s">
+    <row r="184" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C184" s="4" t="s">
         <v>294</v>
       </c>
       <c r="E184" s="2" t="s">
@@ -4097,72 +3535,72 @@
         <v>292</v>
       </c>
     </row>
-    <row r="185" spans="3:6">
-      <c r="C185" s="1" t="s">
+    <row r="185" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C185" s="4" t="s">
         <v>296</v>
       </c>
       <c r="F185" s="1" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="186" spans="3:6">
-      <c r="C186" s="1" t="s">
+    <row r="186" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C186" s="4" t="s">
         <v>297</v>
       </c>
       <c r="F186" s="1" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="187" spans="3:6">
-      <c r="C187" s="1" t="s">
+    <row r="187" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C187" s="4" t="s">
         <v>298</v>
       </c>
       <c r="F187" s="1" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="188" spans="3:6">
-      <c r="C188" s="1" t="s">
+    <row r="188" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C188" s="4" t="s">
         <v>299</v>
       </c>
       <c r="F188" s="1" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="189" spans="2:6">
-      <c r="B189" s="1" t="s">
+    <row r="189" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B189" s="4" t="s">
         <v>300</v>
       </c>
       <c r="F189" s="1" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="190" spans="3:6">
-      <c r="C190" s="1" t="s">
+    <row r="190" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C190" s="4" t="s">
         <v>301</v>
       </c>
       <c r="F190" s="1" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="191" spans="3:6">
-      <c r="C191" s="1" t="s">
+    <row r="191" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C191" s="4" t="s">
         <v>302</v>
       </c>
       <c r="F191" s="1" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="192" spans="3:6">
-      <c r="C192" s="1" t="s">
+    <row r="192" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C192" s="4" t="s">
         <v>303</v>
       </c>
       <c r="F192" s="1" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="193" spans="3:6">
-      <c r="C193" s="1" t="s">
+    <row r="193" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C193" s="4" t="s">
         <v>304</v>
       </c>
       <c r="E193" s="2" t="s">
@@ -4172,16 +3610,16 @@
         <v>292</v>
       </c>
     </row>
-    <row r="194" spans="2:6">
-      <c r="B194" s="1" t="s">
+    <row r="194" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B194" s="4" t="s">
         <v>306</v>
       </c>
       <c r="F194" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="195" spans="3:6">
-      <c r="C195" s="1" t="s">
+    <row r="195" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C195" s="4" t="s">
         <v>307</v>
       </c>
       <c r="E195" s="2" t="s">
@@ -4191,8 +3629,8 @@
         <v>152</v>
       </c>
     </row>
-    <row r="196" spans="3:6">
-      <c r="C196" s="1" t="s">
+    <row r="196" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C196" s="4" t="s">
         <v>309</v>
       </c>
       <c r="E196" s="2" t="s">
@@ -4202,8 +3640,8 @@
         <v>152</v>
       </c>
     </row>
-    <row r="197" spans="3:6">
-      <c r="C197" s="1" t="s">
+    <row r="197" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C197" s="4" t="s">
         <v>311</v>
       </c>
       <c r="E197" s="2" t="s">
@@ -4213,7 +3651,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="198" spans="4:6">
+    <row r="198" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D198" s="1" t="s">
         <v>313</v>
       </c>
@@ -4224,7 +3662,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="199" ht="28.5" spans="4:6">
+    <row r="199" spans="2:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="D199" s="1" t="s">
         <v>315</v>
       </c>
@@ -4235,7 +3673,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="200" spans="4:6">
+    <row r="200" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D200" s="1" t="s">
         <v>317</v>
       </c>
@@ -4246,8 +3684,8 @@
         <v>152</v>
       </c>
     </row>
-    <row r="201" spans="3:6">
-      <c r="C201" s="1" t="s">
+    <row r="201" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C201" s="4" t="s">
         <v>319</v>
       </c>
       <c r="E201" s="2" t="s">
@@ -4257,8 +3695,8 @@
         <v>152</v>
       </c>
     </row>
-    <row r="202" spans="3:6">
-      <c r="C202" s="1" t="s">
+    <row r="202" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C202" s="4" t="s">
         <v>321</v>
       </c>
       <c r="E202" s="2" t="s">
@@ -4268,8 +3706,8 @@
         <v>152</v>
       </c>
     </row>
-    <row r="203" spans="2:6">
-      <c r="B203" s="1" t="s">
+    <row r="203" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B203" s="4" t="s">
         <v>323</v>
       </c>
       <c r="E203" s="2" t="s">
@@ -4279,7 +3717,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="204" spans="4:6">
+    <row r="204" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D204" s="1" t="s">
         <v>325</v>
       </c>
@@ -4287,7 +3725,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="205" spans="4:6">
+    <row r="205" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D205" s="1" t="s">
         <v>326</v>
       </c>
@@ -4295,8 +3733,8 @@
         <v>292</v>
       </c>
     </row>
-    <row r="206" spans="3:6">
-      <c r="C206" s="1" t="s">
+    <row r="206" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C206" s="4" t="s">
         <v>327</v>
       </c>
       <c r="E206" s="2" t="s">
@@ -4306,8 +3744,8 @@
         <v>292</v>
       </c>
     </row>
-    <row r="207" spans="3:6">
-      <c r="C207" s="1" t="s">
+    <row r="207" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C207" s="4" t="s">
         <v>329</v>
       </c>
       <c r="E207" s="2" t="s">
@@ -4317,8 +3755,8 @@
         <v>292</v>
       </c>
     </row>
-    <row r="208" spans="3:6">
-      <c r="C208" s="1" t="s">
+    <row r="208" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C208" s="4" t="s">
         <v>331</v>
       </c>
       <c r="E208" s="2" t="s">
@@ -4328,8 +3766,8 @@
         <v>292</v>
       </c>
     </row>
-    <row r="209" spans="2:6">
-      <c r="B209" s="1" t="s">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B209" s="4" t="s">
         <v>333</v>
       </c>
       <c r="E209" s="2" t="s">
@@ -4339,8 +3777,8 @@
         <v>159</v>
       </c>
     </row>
-    <row r="210" spans="2:6">
-      <c r="B210" s="1" t="s">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B210" s="4" t="s">
         <v>335</v>
       </c>
       <c r="E210" s="2" t="s">
@@ -4350,16 +3788,16 @@
         <v>152</v>
       </c>
     </row>
-    <row r="211" spans="3:6">
-      <c r="C211" s="1" t="s">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C211" s="4" t="s">
         <v>337</v>
       </c>
       <c r="F211" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="212" spans="3:6">
-      <c r="C212" s="1" t="s">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C212" s="4" t="s">
         <v>338</v>
       </c>
       <c r="E212" s="2" t="s">
@@ -4369,8 +3807,8 @@
         <v>152</v>
       </c>
     </row>
-    <row r="213" spans="3:6">
-      <c r="C213" s="1" t="s">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C213" s="4" t="s">
         <v>340</v>
       </c>
       <c r="E213" s="2" t="s">
@@ -4380,8 +3818,8 @@
         <v>152</v>
       </c>
     </row>
-    <row r="214" spans="3:6">
-      <c r="C214" s="1" t="s">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C214" s="4" t="s">
         <v>342</v>
       </c>
       <c r="E214" s="2" t="s">
@@ -4391,8 +3829,8 @@
         <v>152</v>
       </c>
     </row>
-    <row r="215" spans="3:6">
-      <c r="C215" s="1" t="s">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C215" s="4" t="s">
         <v>344</v>
       </c>
       <c r="E215" s="2" t="s">
@@ -4402,7 +3840,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="216" spans="4:6">
+    <row r="216" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D216" s="1" t="s">
         <v>346</v>
       </c>
@@ -4413,7 +3851,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="217" spans="4:6">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D217" s="1" t="s">
         <v>348</v>
       </c>
@@ -4424,7 +3862,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="218" spans="4:6">
+    <row r="218" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D218" s="1" t="s">
         <v>350</v>
       </c>
@@ -4435,7 +3873,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="219" spans="4:6">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D219" s="1" t="s">
         <v>352</v>
       </c>
@@ -4446,38 +3884,38 @@
         <v>152</v>
       </c>
     </row>
-    <row r="220" spans="1:6">
+    <row r="220" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
         <v>354</v>
       </c>
       <c r="F220" s="1"/>
     </row>
-    <row r="221" spans="2:6">
-      <c r="B221" s="1" t="s">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B221" s="4" t="s">
         <v>355</v>
       </c>
       <c r="F221" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="222" spans="3:6">
-      <c r="C222" s="1" t="s">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C222" s="4" t="s">
         <v>356</v>
       </c>
       <c r="F222" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="223" spans="3:6">
-      <c r="C223" s="1" t="s">
+    <row r="223" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C223" s="4" t="s">
         <v>357</v>
       </c>
       <c r="F223" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="224" spans="2:6">
-      <c r="B224" s="1" t="s">
+    <row r="224" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B224" s="4" t="s">
         <v>358</v>
       </c>
       <c r="E224" s="2" t="s">
@@ -4487,16 +3925,16 @@
         <v>46</v>
       </c>
     </row>
-    <row r="225" spans="3:6">
-      <c r="C225" s="1" t="s">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C225" s="4" t="s">
         <v>360</v>
       </c>
       <c r="F225" s="1" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="226" spans="3:6">
-      <c r="C226" s="1" t="s">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C226" s="4" t="s">
         <v>362</v>
       </c>
       <c r="E226" s="2" t="s">
@@ -4506,8 +3944,8 @@
         <v>152</v>
       </c>
     </row>
-    <row r="227" spans="2:6">
-      <c r="B227" s="1" t="s">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B227" s="4" t="s">
         <v>364</v>
       </c>
       <c r="E227" s="2" t="s">
@@ -4517,24 +3955,24 @@
         <v>46</v>
       </c>
     </row>
-    <row r="228" spans="3:6">
-      <c r="C228" s="1" t="s">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C228" s="4" t="s">
         <v>366</v>
       </c>
       <c r="F228" s="1" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="229" spans="3:6">
-      <c r="C229" s="1" t="s">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C229" s="4" t="s">
         <v>367</v>
       </c>
       <c r="F229" s="1" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="230" spans="3:6">
-      <c r="C230" s="1" t="s">
+    <row r="230" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C230" s="4" t="s">
         <v>368</v>
       </c>
       <c r="E230" s="2" t="s">
@@ -4544,14 +3982,14 @@
         <v>152</v>
       </c>
     </row>
-    <row r="231" spans="1:6">
+    <row r="231" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="s">
         <v>370</v>
       </c>
       <c r="F231" s="1"/>
     </row>
-    <row r="232" spans="2:6">
-      <c r="B232" s="1" t="s">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B232" s="4" t="s">
         <v>371</v>
       </c>
       <c r="E232" s="2" t="s">
@@ -4561,16 +3999,16 @@
         <v>46</v>
       </c>
     </row>
-    <row r="233" spans="3:6">
-      <c r="C233" s="1" t="s">
+    <row r="233" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C233" s="4" t="s">
         <v>373</v>
       </c>
       <c r="F233" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="234" spans="3:6">
-      <c r="C234" s="1" t="s">
+    <row r="234" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C234" s="4" t="s">
         <v>374</v>
       </c>
       <c r="E234" s="2" t="s">
@@ -4580,56 +4018,56 @@
         <v>152</v>
       </c>
     </row>
-    <row r="235" spans="3:6">
-      <c r="C235" s="1" t="s">
+    <row r="235" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C235" s="4" t="s">
         <v>376</v>
       </c>
       <c r="F235" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="236" spans="3:6">
-      <c r="C236" s="1" t="s">
+    <row r="236" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C236" s="4" t="s">
         <v>377</v>
       </c>
       <c r="F236" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="237" spans="2:6">
-      <c r="B237" s="1" t="s">
+    <row r="237" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B237" s="4" t="s">
         <v>378</v>
       </c>
       <c r="F237" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="238" spans="3:6">
-      <c r="C238" s="1" t="s">
+    <row r="238" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C238" s="4" t="s">
         <v>379</v>
       </c>
       <c r="F238" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="239" spans="3:6">
-      <c r="C239" s="1" t="s">
+    <row r="239" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C239" s="4" t="s">
         <v>380</v>
       </c>
       <c r="F239" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="240" spans="2:6">
-      <c r="B240" s="1" t="s">
+    <row r="240" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B240" s="4" t="s">
         <v>381</v>
       </c>
       <c r="F240" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="241" spans="3:6">
-      <c r="C241" s="1" t="s">
+    <row r="241" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C241" s="4" t="s">
         <v>382</v>
       </c>
       <c r="E241" s="2" t="s">
@@ -4639,7 +4077,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="242" spans="4:6">
+    <row r="242" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D242" s="1" t="s">
         <v>384</v>
       </c>
@@ -4647,7 +4085,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="243" spans="4:6">
+    <row r="243" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D243" s="1" t="s">
         <v>385</v>
       </c>
@@ -4655,7 +4093,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="244" spans="4:6">
+    <row r="244" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D244" s="1" t="s">
         <v>386</v>
       </c>
@@ -4663,8 +4101,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="245" spans="3:6">
-      <c r="C245" s="1" t="s">
+    <row r="245" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C245" s="4" t="s">
         <v>387</v>
       </c>
       <c r="E245" s="2" t="s">
@@ -4674,15 +4112,15 @@
         <v>49</v>
       </c>
     </row>
-    <row r="246" spans="3:6">
-      <c r="C246" s="1" t="s">
+    <row r="246" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C246" s="4" t="s">
         <v>389</v>
       </c>
       <c r="F246" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="247" spans="3:6">
+    <row r="247" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C247" s="4" t="s">
         <v>390</v>
       </c>
@@ -4693,7 +4131,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="248" spans="4:6">
+    <row r="248" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D248" s="1" t="s">
         <v>393</v>
       </c>
@@ -4701,7 +4139,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="249" spans="4:6">
+    <row r="249" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D249" s="1" t="s">
         <v>395</v>
       </c>
@@ -4709,7 +4147,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="250" spans="4:6">
+    <row r="250" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D250" s="1" t="s">
         <v>396</v>
       </c>
@@ -4717,7 +4155,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="251" spans="4:6">
+    <row r="251" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D251" s="1" t="s">
         <v>397</v>
       </c>
@@ -4728,7 +4166,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="252" spans="4:6">
+    <row r="252" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D252" s="1" t="s">
         <v>399</v>
       </c>
@@ -4736,7 +4174,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="253" spans="4:6">
+    <row r="253" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D253" s="1" t="s">
         <v>400</v>
       </c>
@@ -4747,12 +4185,12 @@
         <v>394</v>
       </c>
     </row>
-    <row r="254" spans="2:2">
-      <c r="B254" s="1" t="s">
+    <row r="254" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B254" s="4" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="255" spans="3:6">
+    <row r="255" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C255" s="4" t="s">
         <v>403</v>
       </c>
@@ -4760,7 +4198,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="256" spans="4:6">
+    <row r="256" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D256" s="1" t="s">
         <v>405</v>
       </c>
@@ -4771,7 +4209,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="257" spans="4:6">
+    <row r="257" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D257" s="1" t="s">
         <v>407</v>
       </c>
@@ -4782,7 +4220,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="258" spans="4:6">
+    <row r="258" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D258" s="1" t="s">
         <v>409</v>
       </c>
@@ -4790,7 +4228,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="259" spans="4:6">
+    <row r="259" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D259" s="1" t="s">
         <v>410</v>
       </c>
@@ -4798,7 +4236,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="260" spans="4:6">
+    <row r="260" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D260" s="1" t="s">
         <v>411</v>
       </c>
@@ -4806,7 +4244,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="261" spans="4:6">
+    <row r="261" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D261" s="1" t="s">
         <v>412</v>
       </c>
@@ -4814,7 +4252,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="262" spans="4:6">
+    <row r="262" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D262" s="1" t="s">
         <v>413</v>
       </c>
@@ -4825,17 +4263,17 @@
         <v>192</v>
       </c>
     </row>
-    <row r="263" spans="2:2">
-      <c r="B263" s="1" t="s">
+    <row r="263" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B263" s="4" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="264" spans="3:3">
-      <c r="C264" s="1" t="s">
+    <row r="264" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C264" s="4" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="265" spans="4:6">
+    <row r="265" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D265" s="1" t="s">
         <v>417</v>
       </c>
@@ -4846,7 +4284,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="266" spans="4:6">
+    <row r="266" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D266" s="1" t="s">
         <v>420</v>
       </c>
@@ -4854,7 +4292,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="267" spans="4:6">
+    <row r="267" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D267" s="1" t="s">
         <v>421</v>
       </c>
@@ -4862,7 +4300,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="268" spans="4:6">
+    <row r="268" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D268" s="1" t="s">
         <v>422</v>
       </c>
@@ -4873,7 +4311,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="269" spans="4:6">
+    <row r="269" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D269" s="1" t="s">
         <v>424</v>
       </c>
@@ -4884,7 +4322,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="270" spans="4:6">
+    <row r="270" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D270" s="1" t="s">
         <v>426</v>
       </c>
@@ -4892,7 +4330,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="271" spans="4:6">
+    <row r="271" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D271" s="1" t="s">
         <v>427</v>
       </c>
@@ -4900,12 +4338,12 @@
         <v>419</v>
       </c>
     </row>
-    <row r="272" spans="3:3">
-      <c r="C272" s="1" t="s">
+    <row r="272" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C272" s="4" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="273" spans="4:6">
+    <row r="273" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D273" s="1" t="s">
         <v>428</v>
       </c>
@@ -4913,7 +4351,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="274" spans="4:6">
+    <row r="274" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D274" s="1" t="s">
         <v>429</v>
       </c>
@@ -4921,45 +4359,45 @@
         <v>419</v>
       </c>
     </row>
-    <row r="275" spans="3:6">
-      <c r="C275" s="1" t="s">
+    <row r="275" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C275" s="4" t="s">
         <v>430</v>
       </c>
       <c r="F275" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="276" spans="3:6">
-      <c r="C276" s="1" t="s">
+    <row r="276" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C276" s="4" t="s">
         <v>431</v>
       </c>
       <c r="F276" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="277" spans="3:6">
-      <c r="C277" s="1" t="s">
+    <row r="277" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C277" s="4" t="s">
         <v>432</v>
       </c>
       <c r="F277" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="278" spans="3:6">
-      <c r="C278" s="1" t="s">
+    <row r="278" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C278" s="4" t="s">
         <v>433</v>
       </c>
       <c r="F278" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="279" spans="2:2">
-      <c r="B279" s="1" t="s">
+    <row r="279" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B279" s="4" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="280" spans="3:6">
-      <c r="C280" s="1" t="s">
+    <row r="280" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C280" s="4" t="s">
         <v>435</v>
       </c>
       <c r="E280" s="2" t="s">
@@ -4969,7 +4407,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="281" spans="4:6">
+    <row r="281" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D281" s="1" t="s">
         <v>437</v>
       </c>
@@ -4977,122 +4415,149 @@
         <v>419</v>
       </c>
     </row>
-    <row r="282" spans="4:6">
+    <row r="282" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D282" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="E282" s="2" t="s">
-        <v>439</v>
+      <c r="E282" s="7" t="s">
+        <v>454</v>
       </c>
       <c r="F282" s="1" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="283" spans="3:6">
-      <c r="C283" s="1" t="s">
-        <v>440</v>
+    <row r="283" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C283" s="4" t="s">
+        <v>439</v>
       </c>
       <c r="F283" s="1" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="284" spans="3:6">
-      <c r="C284" s="1" t="s">
+    <row r="284" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C284" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="F284" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="F284" s="1" t="s">
+    </row>
+    <row r="285" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C285" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="285" spans="3:6">
-      <c r="C285" s="1" t="s">
+      <c r="F285" s="1" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="286" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B286" s="4" t="s">
         <v>443</v>
       </c>
-      <c r="F285" s="1" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="286" spans="2:6">
-      <c r="B286" s="1" t="s">
+      <c r="F286" s="1"/>
+    </row>
+    <row r="287" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C287" s="4" t="s">
         <v>444</v>
-      </c>
-      <c r="F286" s="1"/>
-    </row>
-    <row r="287" spans="3:6">
-      <c r="C287" s="1" t="s">
-        <v>445</v>
       </c>
       <c r="F287" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="288" spans="4:6">
+    <row r="288" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D288" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F288" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="289" spans="4:6">
+    <row r="289" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D289" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="F289" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="290" spans="4:6">
+    <row r="290" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D290" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="F290" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="291" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C291" s="4" t="s">
         <v>448</v>
-      </c>
-      <c r="F290" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="291" spans="3:6">
-      <c r="C291" s="1" t="s">
-        <v>449</v>
       </c>
       <c r="F291" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="292" spans="4:6">
+    <row r="292" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D292" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F292" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="293" spans="4:6">
+    <row r="293" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D293" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="F293" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="294" spans="4:6">
+    <row r="294" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D294" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F294" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="295" spans="4:6">
+    <row r="295" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D295" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="F295" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="296" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A296" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="F295" s="1" t="s">
-        <v>152</v>
+      <c r="D296" s="8" t="s">
+        <v>455</v>
+      </c>
+      <c r="E296" s="7" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="297" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D297" s="8" t="s">
+        <v>456</v>
+      </c>
+      <c r="E297" s="7" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="298" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D298" s="8" t="s">
+        <v>457</v>
+      </c>
+      <c r="E298" s="7" t="s">
+        <v>459</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>
-  <headerFooter/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Feature/thafpm fix bug 20211228 (#1341)
* should not be added code

* fix bug

* file change

* fix bug

* file change

* De-duplicate the door

Co-authored-by: THAPE\tiankaihe <1204973192@qq.com>
</commit_message>
<xml_diff>
--- a/AutoLoader/Contents/Support/房间名称分类处理.xlsx
+++ b/AutoLoader/Contents/Support/房间名称分类处理.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2044" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2044" uniqueCount="540">
   <si>
     <t>一级</t>
   </si>
@@ -202,7 +202,7 @@
     <t>*阳台</t>
   </si>
   <si>
-    <t>私有区域；非火灾探测区域；消防广播需要保护；声光手报需要保护</t>
+    <t>私有区域；非火灾探测区域；正常照明；消防广播需要保护；声光手报需要保护</t>
   </si>
   <si>
     <t>公共场所</t>
@@ -1213,15 +1213,12 @@
     <t>非机动车停车场</t>
   </si>
   <si>
-    <t>汽车库</t>
-  </si>
-  <si>
-    <t>停车库，车库，I类汽车库，II类汽车库，机动车库</t>
-  </si>
-  <si>
     <t>机动车库</t>
   </si>
   <si>
+    <t>停车库，车库，I类汽车库，II类汽车库，汽车库</t>
+  </si>
+  <si>
     <t>地下车库</t>
   </si>
   <si>
@@ -1331,9 +1328,6 @@
   </si>
   <si>
     <t>无障碍盆浴间</t>
-  </si>
-  <si>
-    <t>私有区域；非火灾探测区域；正常照明；消防广播需要保护；声光手报需要保护</t>
   </si>
   <si>
     <t>无障碍淋浴间</t>
@@ -1651,41 +1645,41 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="36">
     <numFmt numFmtId="176" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;"/>
+    <numFmt numFmtId="6" formatCode="&quot;￥&quot;#,##0;[Red]&quot;￥&quot;\-#,##0"/>
     <numFmt numFmtId="23" formatCode="\$#,##0_);\(\$#,##0\)"/>
-    <numFmt numFmtId="177" formatCode="#\ ??/??"/>
-    <numFmt numFmtId="178" formatCode="mmmm\-yy"/>
+    <numFmt numFmtId="177" formatCode="mmmm\-yy"/>
     <numFmt numFmtId="5" formatCode="&quot;￥&quot;#,##0;&quot;￥&quot;\-#,##0"/>
-    <numFmt numFmtId="179" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;"/>
-    <numFmt numFmtId="180" formatCode="[$-804]aaa"/>
-    <numFmt numFmtId="181" formatCode="mmmmm"/>
-    <numFmt numFmtId="182" formatCode="\¥#,##0;[Red]\¥\-#,##0"/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="183" formatCode="[DBNum1]上午/下午h&quot;时&quot;mm&quot;分&quot;"/>
-    <numFmt numFmtId="184" formatCode="[DBNum1][$-804]m&quot;月&quot;d&quot;日&quot;"/>
-    <numFmt numFmtId="185" formatCode="[$-804]aaaa"/>
-    <numFmt numFmtId="186" formatCode="\¥#,##0.00;[Red]\¥\-#,##0.00"/>
-    <numFmt numFmtId="187" formatCode="\¥#,##0.00;\¥\-#,##0.00"/>
-    <numFmt numFmtId="188" formatCode="yyyy/m/d\ h:mm\ AM/PM"/>
+    <numFmt numFmtId="178" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;"/>
+    <numFmt numFmtId="179" formatCode="[$-804]aaa"/>
+    <numFmt numFmtId="180" formatCode="h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="181" formatCode="[$-804]aaaa"/>
+    <numFmt numFmtId="182" formatCode="yyyy/m/d\ h:mm\ AM/PM"/>
+    <numFmt numFmtId="8" formatCode="&quot;￥&quot;#,##0.00;[Red]&quot;￥&quot;\-#,##0.00"/>
+    <numFmt numFmtId="183" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="25" formatCode="\$#,##0.00_);\(\$#,##0.00\)"/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="184" formatCode="h:mm\ AM/PM"/>
+    <numFmt numFmtId="185" formatCode="dd\-mmm\-yy"/>
+    <numFmt numFmtId="186" formatCode="mmmmm\-yy"/>
+    <numFmt numFmtId="187" formatCode="\¥#,##0.00;[Red]\¥\-#,##0.00"/>
+    <numFmt numFmtId="24" formatCode="\$#,##0_);[Red]\(\$#,##0\)"/>
+    <numFmt numFmtId="188" formatCode="m/d"/>
     <numFmt numFmtId="26" formatCode="\$#,##0.00_);[Red]\(\$#,##0.00\)"/>
-    <numFmt numFmtId="189" formatCode="yy/m/d"/>
-    <numFmt numFmtId="6" formatCode="&quot;￥&quot;#,##0;[Red]&quot;￥&quot;\-#,##0"/>
+    <numFmt numFmtId="189" formatCode="[DBNum1]h&quot;时&quot;mm&quot;分&quot;"/>
     <numFmt numFmtId="190" formatCode="#\ ?/?"/>
-    <numFmt numFmtId="191" formatCode="dd\-mmm\-yy"/>
-    <numFmt numFmtId="25" formatCode="\$#,##0.00_);\(\$#,##0.00\)"/>
-    <numFmt numFmtId="192" formatCode="\¥#,##0;\¥\-#,##0"/>
-    <numFmt numFmtId="193" formatCode="mm/dd/yy"/>
-    <numFmt numFmtId="194" formatCode="mmmmm\-yy"/>
+    <numFmt numFmtId="191" formatCode="mmmmm"/>
+    <numFmt numFmtId="192" formatCode="#\ ??/??"/>
+    <numFmt numFmtId="193" formatCode="[DBNum1]上午/下午h&quot;时&quot;mm&quot;分&quot;"/>
+    <numFmt numFmtId="194" formatCode="\¥#,##0;\¥\-#,##0"/>
+    <numFmt numFmtId="195" formatCode="\¥#,##0;[Red]\¥\-#,##0"/>
+    <numFmt numFmtId="196" formatCode="\¥#,##0.00;\¥\-#,##0.00"/>
+    <numFmt numFmtId="197" formatCode="#\ ??"/>
+    <numFmt numFmtId="198" formatCode="[DBNum1][$-804]m&quot;月&quot;d&quot;日&quot;"/>
     <numFmt numFmtId="7" formatCode="&quot;￥&quot;#,##0.00;&quot;￥&quot;\-#,##0.00"/>
-    <numFmt numFmtId="195" formatCode="m/d"/>
-    <numFmt numFmtId="8" formatCode="&quot;￥&quot;#,##0.00;[Red]&quot;￥&quot;\-#,##0.00"/>
-    <numFmt numFmtId="196" formatCode="h:mm\ AM/PM"/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="197" formatCode="[DBNum1]h&quot;时&quot;mm&quot;分&quot;"/>
-    <numFmt numFmtId="198" formatCode="h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="199" formatCode="#\ ??"/>
-    <numFmt numFmtId="24" formatCode="\$#,##0_);[Red]\(\$#,##0\)"/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="199" formatCode="yy/m/d"/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -1724,62 +1718,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1801,8 +1740,63 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1810,6 +1804,22 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1823,31 +1833,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1874,13 +1868,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1892,25 +1886,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1922,37 +1928,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1964,37 +1940,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2012,7 +1958,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2024,13 +2000,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2042,13 +2018,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2067,6 +2061,17 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2096,16 +2101,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2127,17 +2132,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
@@ -2146,158 +2140,158 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2677,7 +2671,7 @@
   <dimension ref="A1:P318"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="O1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A298" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A211" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="O306" sqref="O306"/>
     </sheetView>
@@ -3106,7 +3100,7 @@
       <c r="E24" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F24" s="8" t="s">
         <v>61</v>
       </c>
       <c r="I24" s="9" t="s">
@@ -7668,17 +7662,17 @@
       </c>
     </row>
     <row r="229" spans="2:10">
-      <c r="B229" s="1" t="s">
+      <c r="B229" s="12" t="s">
         <v>398</v>
       </c>
-      <c r="E229" s="2" t="s">
+      <c r="E229" s="8" t="s">
         <v>399</v>
       </c>
       <c r="F229" s="2" t="s">
         <v>97</v>
       </c>
       <c r="H229" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="I229" s="9" t="s">
         <v>23</v>
@@ -7689,13 +7683,13 @@
     </row>
     <row r="230" spans="3:14">
       <c r="C230" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F230" s="8" t="s">
         <v>97</v>
       </c>
       <c r="H230" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="I230" s="9" t="s">
         <v>23</v>
@@ -7710,13 +7704,13 @@
     </row>
     <row r="231" spans="3:14">
       <c r="C231" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="E231" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="E231" s="2" t="s">
+      <c r="F231" s="2" t="s">
         <v>403</v>
-      </c>
-      <c r="F231" s="2" t="s">
-        <v>404</v>
       </c>
       <c r="I231" s="9" t="s">
         <v>23</v>
@@ -7733,16 +7727,16 @@
     </row>
     <row r="232" spans="2:10">
       <c r="B232" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="E232" s="2" t="s">
         <v>405</v>
-      </c>
-      <c r="E232" s="2" t="s">
-        <v>406</v>
       </c>
       <c r="F232" s="2" t="s">
         <v>97</v>
       </c>
       <c r="H232" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="I232" s="9" t="s">
         <v>23</v>
@@ -7753,13 +7747,13 @@
     </row>
     <row r="233" spans="3:11">
       <c r="C233" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="F233" s="8" t="s">
         <v>97</v>
       </c>
       <c r="H233" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="I233" s="9" t="s">
         <v>23</v>
@@ -7773,13 +7767,13 @@
     </row>
     <row r="234" spans="3:11">
       <c r="C234" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F234" s="8" t="s">
         <v>97</v>
       </c>
       <c r="H234" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="I234" s="9" t="s">
         <v>23</v>
@@ -7793,16 +7787,16 @@
     </row>
     <row r="235" spans="3:14">
       <c r="C235" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="E235" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="E235" s="2" t="s">
-        <v>410</v>
-      </c>
       <c r="F235" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="H235" t="s">
         <v>404</v>
-      </c>
-      <c r="H235" t="s">
-        <v>405</v>
       </c>
       <c r="I235" s="9" t="s">
         <v>23</v>
@@ -7819,7 +7813,7 @@
     </row>
     <row r="236" spans="1:10">
       <c r="A236" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F236" s="2"/>
       <c r="I236" s="9" t="s">
@@ -7831,7 +7825,7 @@
     </row>
     <row r="237" spans="2:14">
       <c r="B237" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F237" s="2"/>
       <c r="I237" s="9"/>
@@ -7845,13 +7839,13 @@
     </row>
     <row r="238" spans="3:14">
       <c r="C238" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="E238" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="E238" s="2" t="s">
-        <v>414</v>
-      </c>
       <c r="F238" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="I238" s="9" t="s">
         <v>23</v>
@@ -7868,16 +7862,16 @@
     </row>
     <row r="239" spans="3:14">
       <c r="C239" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="E239" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="E239" s="2" t="s">
+      <c r="F239" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="H239" t="s">
         <v>416</v>
-      </c>
-      <c r="F239" s="2" t="s">
-        <v>404</v>
-      </c>
-      <c r="H239" t="s">
-        <v>417</v>
       </c>
       <c r="I239" s="9" t="s">
         <v>23</v>
@@ -7894,13 +7888,13 @@
     </row>
     <row r="240" spans="3:14">
       <c r="C240" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F240" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="H240" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="I240" s="9" t="s">
         <v>23</v>
@@ -7917,10 +7911,10 @@
     </row>
     <row r="241" spans="3:14">
       <c r="C241" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="F241" s="2" t="s">
         <v>419</v>
-      </c>
-      <c r="F241" s="2" t="s">
-        <v>420</v>
       </c>
       <c r="I241" s="9" t="s">
         <v>67</v>
@@ -7937,7 +7931,7 @@
     </row>
     <row r="242" spans="2:14">
       <c r="B242" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F242" s="2"/>
       <c r="K242" s="9" t="s">
@@ -7949,10 +7943,10 @@
     </row>
     <row r="243" spans="3:14">
       <c r="C243" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F243" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="I243" s="9" t="s">
         <v>23</v>
@@ -7969,10 +7963,10 @@
     </row>
     <row r="244" spans="3:14">
       <c r="C244" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F244" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="I244" s="9" t="s">
         <v>23</v>
@@ -7989,7 +7983,7 @@
     </row>
     <row r="245" spans="2:14">
       <c r="B245" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F245" s="2"/>
       <c r="K245" s="9" t="s">
@@ -8001,13 +7995,13 @@
     </row>
     <row r="246" spans="3:14">
       <c r="C246" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E246" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="E246" s="2" t="s">
+      <c r="F246" s="2" t="s">
         <v>426</v>
-      </c>
-      <c r="F246" s="2" t="s">
-        <v>427</v>
       </c>
       <c r="I246" s="9" t="s">
         <v>23</v>
@@ -8024,10 +8018,10 @@
     </row>
     <row r="247" spans="4:14">
       <c r="D247" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="F247" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="I247" s="9" t="s">
         <v>23</v>
@@ -8044,7 +8038,7 @@
     </row>
     <row r="248" ht="28.5" spans="4:14">
       <c r="D248" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F248" s="2" t="s">
         <v>30</v>
@@ -8064,7 +8058,7 @@
     </row>
     <row r="249" ht="28.5" spans="4:16">
       <c r="D249" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F249" s="2" t="s">
         <v>89</v>
@@ -8090,10 +8084,10 @@
     </row>
     <row r="250" ht="28.5" spans="3:16">
       <c r="C250" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="E250" s="2" t="s">
         <v>431</v>
-      </c>
-      <c r="E250" s="2" t="s">
-        <v>432</v>
       </c>
       <c r="F250" s="8" t="s">
         <v>76</v>
@@ -8119,10 +8113,10 @@
     </row>
     <row r="251" spans="3:14">
       <c r="C251" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F251" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="I251" s="9" t="s">
         <v>23</v>
@@ -8139,13 +8133,13 @@
     </row>
     <row r="252" spans="3:11">
       <c r="C252" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="E252" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="E252" s="2" t="s">
+      <c r="F252" s="8" t="s">
         <v>435</v>
-      </c>
-      <c r="F252" s="8" t="s">
-        <v>436</v>
       </c>
       <c r="I252" s="9" t="s">
         <v>67</v>
@@ -8159,10 +8153,10 @@
     </row>
     <row r="253" spans="4:11">
       <c r="D253" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F253" s="2" t="s">
-        <v>438</v>
+        <v>61</v>
       </c>
       <c r="I253" s="9" t="s">
         <v>67</v>
@@ -8176,10 +8170,10 @@
     </row>
     <row r="254" spans="4:11">
       <c r="D254" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="F254" s="2" t="s">
-        <v>438</v>
+        <v>61</v>
       </c>
       <c r="I254" s="9" t="s">
         <v>67</v>
@@ -8193,10 +8187,10 @@
     </row>
     <row r="255" spans="4:11">
       <c r="D255" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="F255" s="2" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="I255" s="9" t="s">
         <v>67</v>
@@ -8210,13 +8204,13 @@
     </row>
     <row r="256" spans="4:11">
       <c r="D256" s="1" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="E256" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="F256" s="2" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="I256" s="9" t="s">
         <v>67</v>
@@ -8230,10 +8224,10 @@
     </row>
     <row r="257" ht="28.5" spans="4:11">
       <c r="D257" s="1" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F257" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="I257" s="9" t="s">
         <v>67</v>
@@ -8247,13 +8241,13 @@
     </row>
     <row r="258" spans="4:11">
       <c r="D258" s="1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E258" s="2" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="F258" s="2" t="s">
-        <v>438</v>
+        <v>61</v>
       </c>
       <c r="I258" s="9" t="s">
         <v>67</v>
@@ -8267,7 +8261,7 @@
     </row>
     <row r="259" spans="1:11">
       <c r="A259" s="1" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="I259" s="9"/>
       <c r="J259" s="9"/>
@@ -8275,7 +8269,7 @@
     </row>
     <row r="260" spans="2:11">
       <c r="B260" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="F260" s="2"/>
       <c r="I260" s="9"/>
@@ -8284,13 +8278,13 @@
     </row>
     <row r="261" spans="3:11">
       <c r="C261" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="E261" s="2" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="F261" s="2" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="I261" s="9" t="s">
         <v>67</v>
@@ -8304,13 +8298,13 @@
     </row>
     <row r="262" spans="3:11">
       <c r="C262" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="E262" s="2" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="F262" s="2" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="I262" s="9" t="s">
         <v>67</v>
@@ -8324,10 +8318,10 @@
     </row>
     <row r="263" ht="28.5" spans="3:13">
       <c r="C263" s="1" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="F263" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="I263" s="9" t="s">
         <v>67</v>
@@ -8344,10 +8338,10 @@
     </row>
     <row r="264" spans="3:13">
       <c r="C264" s="1" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="F264" s="2" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="I264" s="9" t="s">
         <v>67</v>
@@ -8362,10 +8356,10 @@
     </row>
     <row r="265" spans="3:11">
       <c r="C265" s="1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="F265" s="2" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="I265" s="9" t="s">
         <v>67</v>
@@ -8382,7 +8376,7 @@
         <v>108</v>
       </c>
       <c r="F266" s="2" t="s">
-        <v>438</v>
+        <v>61</v>
       </c>
       <c r="I266" s="9" t="s">
         <v>67</v>
@@ -8394,10 +8388,10 @@
     </row>
     <row r="267" spans="3:11">
       <c r="C267" s="12" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E267" s="2" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="F267" s="2" t="s">
         <v>211</v>
@@ -8414,7 +8408,7 @@
     </row>
     <row r="268" spans="1:11">
       <c r="A268" s="1" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="F268" s="2"/>
       <c r="I268" s="9"/>
@@ -8423,10 +8417,10 @@
     </row>
     <row r="269" spans="2:10">
       <c r="B269" s="1" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="H269" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="I269" s="9" t="s">
         <v>67</v>
@@ -8437,16 +8431,16 @@
     </row>
     <row r="270" ht="28.5" spans="3:16">
       <c r="C270" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="E270" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="F270" s="3" t="s">
         <v>461</v>
       </c>
-      <c r="E270" s="2" t="s">
-        <v>462</v>
-      </c>
-      <c r="F270" s="3" t="s">
-        <v>463</v>
-      </c>
       <c r="H270" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="I270" s="9" t="s">
         <v>67</v>
@@ -8466,13 +8460,13 @@
     </row>
     <row r="271" ht="28.5" spans="3:16">
       <c r="C271" s="1" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="F271" s="2" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="H271" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="I271" s="9" t="s">
         <v>67</v>
@@ -8492,13 +8486,13 @@
     </row>
     <row r="272" ht="28.5" spans="3:16">
       <c r="C272" s="1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="F272" s="2" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="H272" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="I272" s="9" t="s">
         <v>67</v>
@@ -8518,13 +8512,13 @@
     </row>
     <row r="273" ht="28.5" spans="3:16">
       <c r="C273" s="1" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="E273" s="2" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="F273" s="2" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="H273" t="s">
         <v>167</v>
@@ -8547,16 +8541,16 @@
     </row>
     <row r="274" ht="28.5" spans="3:16">
       <c r="C274" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="E274" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="F274" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="H274" t="s">
         <v>468</v>
-      </c>
-      <c r="E274" s="2" t="s">
-        <v>469</v>
-      </c>
-      <c r="F274" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="H274" t="s">
-        <v>470</v>
       </c>
       <c r="I274" s="9" t="s">
         <v>67</v>
@@ -8576,10 +8570,10 @@
     </row>
     <row r="275" ht="28.5" spans="3:16">
       <c r="C275" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="F275" s="2" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="I275" s="9" t="s">
         <v>67</v>
@@ -8599,13 +8593,13 @@
     </row>
     <row r="276" ht="28.5" spans="3:16">
       <c r="C276" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="F276" s="2" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="H276" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="I276" s="9" t="s">
         <v>67</v>
@@ -8625,12 +8619,12 @@
     </row>
     <row r="277" spans="2:16">
       <c r="B277" s="1" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C277" s="1"/>
       <c r="F277" s="2"/>
       <c r="H277" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="I277" s="9" t="s">
         <v>67</v>
@@ -8644,13 +8638,13 @@
     </row>
     <row r="278" ht="28.5" spans="3:16">
       <c r="C278" s="1" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="F278" s="3" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="H278" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="I278" s="9" t="s">
         <v>67</v>
@@ -8670,13 +8664,13 @@
     </row>
     <row r="279" ht="28.5" spans="3:16">
       <c r="C279" s="1" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="F279" s="2" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="H279" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="I279" s="9" t="s">
         <v>67</v>
@@ -8696,13 +8690,13 @@
     </row>
     <row r="280" ht="28.5" spans="3:16">
       <c r="C280" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="F280" s="2" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="H280" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="I280" s="9" t="s">
         <v>67</v>
@@ -8716,13 +8710,13 @@
     </row>
     <row r="281" ht="28.5" spans="3:10">
       <c r="C281" s="1" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="F281" s="2" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="H281" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="I281" s="9" t="s">
         <v>67</v>
@@ -8733,14 +8727,14 @@
     </row>
     <row r="282" spans="2:11">
       <c r="B282" s="1" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C282" s="1"/>
       <c r="F282" s="2" t="s">
         <v>97</v>
       </c>
       <c r="H282" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="I282" s="9" t="s">
         <v>23</v>
@@ -8754,7 +8748,7 @@
     </row>
     <row r="283" spans="2:15">
       <c r="B283" s="1" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="F283" s="2" t="s">
         <v>97</v>
@@ -8772,7 +8766,7 @@
     </row>
     <row r="284" ht="28.5" spans="2:16">
       <c r="B284" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="F284" s="2" t="s">
         <v>105</v>
@@ -8798,16 +8792,16 @@
     </row>
     <row r="285" spans="2:16">
       <c r="B285" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="E285" s="8" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="F285" s="8" t="s">
         <v>32</v>
       </c>
       <c r="H285" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="I285" s="9" t="s">
         <v>28</v>
@@ -8821,16 +8815,16 @@
     </row>
     <row r="286" spans="2:11">
       <c r="B286" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="E286" s="2" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="F286" s="2" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="H286" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="I286" s="9" t="s">
         <v>67</v>
@@ -8844,7 +8838,7 @@
     </row>
     <row r="287" spans="1:11">
       <c r="A287" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B287" s="1"/>
       <c r="F287" s="2"/>
@@ -8856,16 +8850,16 @@
     </row>
     <row r="288" ht="28.5" spans="2:16">
       <c r="B288" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="E288" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="F288" s="3" t="s">
         <v>486</v>
       </c>
-      <c r="E288" s="2" t="s">
-        <v>487</v>
-      </c>
-      <c r="F288" s="3" t="s">
-        <v>488</v>
-      </c>
       <c r="H288" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="I288" s="5" t="s">
         <v>23</v>
@@ -8885,16 +8879,16 @@
     </row>
     <row r="289" ht="28.5" spans="3:16">
       <c r="C289" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="E289" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="F289" s="2" t="s">
         <v>489</v>
       </c>
-      <c r="E289" s="2" t="s">
-        <v>490</v>
-      </c>
-      <c r="F289" s="2" t="s">
-        <v>491</v>
-      </c>
       <c r="H289" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="I289" s="9" t="s">
         <v>23</v>
@@ -8917,16 +8911,16 @@
     </row>
     <row r="290" ht="28.5" spans="3:16">
       <c r="C290" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="E290" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="F290" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="H290" t="s">
         <v>492</v>
-      </c>
-      <c r="E290" s="2" t="s">
-        <v>493</v>
-      </c>
-      <c r="F290" s="2" t="s">
-        <v>488</v>
-      </c>
-      <c r="H290" t="s">
-        <v>494</v>
       </c>
       <c r="I290" s="9" t="s">
         <v>23</v>
@@ -8947,17 +8941,17 @@
     </row>
     <row r="291" ht="28.5" spans="2:16">
       <c r="B291" s="1" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C291" s="1"/>
       <c r="E291" s="8" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="F291" s="2" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="H291" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="I291" s="9" t="s">
         <v>23</v>
@@ -8977,13 +8971,13 @@
     </row>
     <row r="292" ht="28.5" spans="2:16">
       <c r="B292" s="1" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="F292" s="2" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="H292" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="I292" s="9" t="s">
         <v>23</v>
@@ -9003,10 +8997,10 @@
     </row>
     <row r="293" ht="28.5" spans="2:16">
       <c r="B293" s="1" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="F293" s="2" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="H293" t="s">
         <v>102</v>
@@ -9029,13 +9023,13 @@
     </row>
     <row r="294" spans="2:16">
       <c r="B294" s="1" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="F294" s="2" t="s">
         <v>204</v>
       </c>
       <c r="H294" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="I294" s="9" t="s">
         <v>67</v>
@@ -9051,13 +9045,13 @@
     </row>
     <row r="295" spans="2:15">
       <c r="B295" s="1" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F295" s="8" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="H295" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="I295" s="9" t="s">
         <v>67</v>
@@ -9072,13 +9066,13 @@
     </row>
     <row r="296" ht="28.5" spans="2:16">
       <c r="B296" s="1" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="F296" s="8" t="s">
         <v>105</v>
       </c>
       <c r="H296" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="I296" s="9" t="s">
         <v>23</v>
@@ -9098,16 +9092,16 @@
     </row>
     <row r="297" ht="28.5" spans="2:16">
       <c r="B297" s="1" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="E297" s="2" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="F297" s="2" t="s">
         <v>105</v>
       </c>
       <c r="H297" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="I297" s="9" t="s">
         <v>23</v>
@@ -9127,16 +9121,16 @@
     </row>
     <row r="298" ht="28.5" spans="2:16">
       <c r="B298" s="1" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="E298" s="2" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="F298" s="2" t="s">
         <v>105</v>
       </c>
       <c r="H298" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="I298" s="9" t="s">
         <v>23</v>
@@ -9156,16 +9150,16 @@
     </row>
     <row r="299" ht="28.5" spans="2:16">
       <c r="B299" s="1" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="E299" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="F299" s="2" t="s">
         <v>105</v>
       </c>
       <c r="H299" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="I299" s="9" t="s">
         <v>23</v>
@@ -9185,16 +9179,16 @@
     </row>
     <row r="300" ht="28.5" spans="2:16">
       <c r="B300" s="1" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E300" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="F300" s="2" t="s">
         <v>105</v>
       </c>
       <c r="H300" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="I300" s="9" t="s">
         <v>23</v>
@@ -9214,7 +9208,7 @@
     </row>
     <row r="301" spans="1:16">
       <c r="A301" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="B301" s="1"/>
       <c r="F301" s="2"/>
@@ -9228,7 +9222,7 @@
     </row>
     <row r="302" ht="28.5" spans="2:11">
       <c r="B302" s="1" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="F302" s="2" t="s">
         <v>105</v>
@@ -9245,16 +9239,16 @@
     </row>
     <row r="303" ht="28.5" spans="3:16">
       <c r="C303" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="E303" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="F303" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="H303" t="s">
         <v>515</v>
-      </c>
-      <c r="E303" s="2" t="s">
-        <v>516</v>
-      </c>
-      <c r="F303" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="H303" t="s">
-        <v>517</v>
       </c>
       <c r="I303" s="9" t="s">
         <v>23</v>
@@ -9274,16 +9268,16 @@
     </row>
     <row r="304" ht="28.5" spans="3:16">
       <c r="C304" s="1" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="E304" s="2" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F304" s="2" t="s">
         <v>105</v>
       </c>
       <c r="H304" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="I304" s="9" t="s">
         <v>23</v>
@@ -9303,13 +9297,13 @@
     </row>
     <row r="305" ht="28.5" spans="3:16">
       <c r="C305" s="1" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="F305" s="2" t="s">
         <v>105</v>
       </c>
       <c r="H305" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="I305" s="9" t="s">
         <v>23</v>
@@ -9325,16 +9319,16 @@
     </row>
     <row r="306" spans="3:16">
       <c r="C306" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="E306" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="F306" s="8" t="s">
         <v>522</v>
       </c>
-      <c r="E306" s="2" t="s">
+      <c r="H306" t="s">
         <v>523</v>
-      </c>
-      <c r="F306" s="8" t="s">
-        <v>524</v>
-      </c>
-      <c r="H306" t="s">
-        <v>525</v>
       </c>
       <c r="I306" s="9" t="s">
         <v>23</v>
@@ -9353,16 +9347,16 @@
     </row>
     <row r="307" ht="28.5" spans="3:16">
       <c r="C307" s="1" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="E307" s="2" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="F307" s="2" t="s">
         <v>105</v>
       </c>
       <c r="H307" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="I307" s="9" t="s">
         <v>23</v>
@@ -9383,7 +9377,7 @@
     </row>
     <row r="308" spans="2:16">
       <c r="B308" s="1" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="C308" s="1"/>
       <c r="F308" s="2"/>
@@ -9397,7 +9391,7 @@
     </row>
     <row r="309" ht="28.5" spans="3:16">
       <c r="C309" s="1" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="F309" s="2" t="s">
         <v>105</v>
@@ -9420,7 +9414,7 @@
     </row>
     <row r="310" ht="28.5" spans="3:16">
       <c r="C310" s="1" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="F310" s="2" t="s">
         <v>105</v>
@@ -9443,7 +9437,7 @@
     </row>
     <row r="311" ht="28.5" spans="3:16">
       <c r="C311" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="F311" s="2" t="s">
         <v>105</v>
@@ -9466,10 +9460,10 @@
     </row>
     <row r="312" spans="3:16">
       <c r="C312" s="1" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="F312" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="I312" s="9" t="s">
         <v>23</v>
@@ -9488,7 +9482,7 @@
     </row>
     <row r="313" spans="1:14">
       <c r="A313" s="1" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="F313" s="2"/>
       <c r="I313" s="9"/>
@@ -9500,7 +9494,7 @@
     </row>
     <row r="314" spans="2:11">
       <c r="B314" s="1" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="F314" s="2"/>
       <c r="K314" s="9" t="s">
@@ -9509,10 +9503,10 @@
     </row>
     <row r="315" ht="28.5" spans="3:16">
       <c r="C315" s="1" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="E315" s="2" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="F315" s="2" t="s">
         <v>105</v>
@@ -9535,10 +9529,10 @@
     </row>
     <row r="316" ht="28.5" spans="3:16">
       <c r="C316" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="E316" s="14" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="F316" s="2" t="s">
         <v>105</v>
@@ -9561,10 +9555,10 @@
     </row>
     <row r="317" ht="28.5" spans="3:16">
       <c r="C317" s="13" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="E317" s="14" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="F317" s="2" t="s">
         <v>105</v>
@@ -9587,13 +9581,13 @@
     </row>
     <row r="318" spans="3:16">
       <c r="C318" s="13" t="s">
+        <v>537</v>
+      </c>
+      <c r="E318" s="14" t="s">
+        <v>538</v>
+      </c>
+      <c r="F318" s="2" t="s">
         <v>539</v>
-      </c>
-      <c r="E318" s="14" t="s">
-        <v>540</v>
-      </c>
-      <c r="F318" s="2" t="s">
-        <v>541</v>
       </c>
       <c r="I318" s="9" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Update Room configuration file 修复了层级断档问题
</commit_message>
<xml_diff>
--- a/AutoLoader/Contents/Support/房间名称分类处理.xlsx
+++ b/AutoLoader/Contents/Support/房间名称分类处理.xlsx
@@ -268,13 +268,13 @@
     <t>消防电梯前室</t>
   </si>
   <si>
-    <t>消防前室，*消防电梯前室*</t>
+    <t>消防前室，*消防电梯前室</t>
   </si>
   <si>
     <t>电梯前室</t>
   </si>
   <si>
-    <t>*电梯前室*</t>
+    <t>*电梯前室</t>
   </si>
   <si>
     <t>合用前室</t>
@@ -1968,42 +1968,42 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="36">
-    <numFmt numFmtId="176" formatCode="\¥#,##0.00;[Red]\¥\-#,##0.00"/>
+    <numFmt numFmtId="176" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;"/>
+    <numFmt numFmtId="6" formatCode="&quot;￥&quot;#,##0;[Red]&quot;￥&quot;\-#,##0"/>
+    <numFmt numFmtId="177" formatCode="\¥#,##0.00;[Red]\¥\-#,##0.00"/>
+    <numFmt numFmtId="23" formatCode="\$#,##0_);\(\$#,##0\)"/>
+    <numFmt numFmtId="178" formatCode="#\ ??/??"/>
+    <numFmt numFmtId="179" formatCode="mmmm\-yy"/>
+    <numFmt numFmtId="5" formatCode="&quot;￥&quot;#,##0;&quot;￥&quot;\-#,##0"/>
     <numFmt numFmtId="24" formatCode="\$#,##0_);[Red]\(\$#,##0\)"/>
-    <numFmt numFmtId="177" formatCode="#\ ?/?"/>
-    <numFmt numFmtId="6" formatCode="&quot;￥&quot;#,##0;[Red]&quot;￥&quot;\-#,##0"/>
+    <numFmt numFmtId="180" formatCode="[DBNum1]上午/下午h&quot;时&quot;mm&quot;分&quot;"/>
+    <numFmt numFmtId="181" formatCode="[$-804]aaa"/>
+    <numFmt numFmtId="8" formatCode="&quot;￥&quot;#,##0.00;[Red]&quot;￥&quot;\-#,##0.00"/>
+    <numFmt numFmtId="182" formatCode="[DBNum1][$-804]m&quot;月&quot;d&quot;日&quot;"/>
+    <numFmt numFmtId="183" formatCode="[$-804]aaaa"/>
+    <numFmt numFmtId="184" formatCode="yyyy/m/d\ h:mm\ AM/PM"/>
+    <numFmt numFmtId="26" formatCode="\$#,##0.00_);[Red]\(\$#,##0.00\)"/>
+    <numFmt numFmtId="185" formatCode="#\ ?/?"/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="186" formatCode="yy/m/d"/>
+    <numFmt numFmtId="187" formatCode="dd\-mmm\-yy"/>
+    <numFmt numFmtId="188" formatCode="\¥#,##0;[Red]\¥\-#,##0"/>
+    <numFmt numFmtId="7" formatCode="&quot;￥&quot;#,##0.00;&quot;￥&quot;\-#,##0.00"/>
+    <numFmt numFmtId="189" formatCode="mmmmm"/>
+    <numFmt numFmtId="190" formatCode="h:mm\ AM/PM"/>
+    <numFmt numFmtId="191" formatCode="h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="192" formatCode="\¥#,##0;\¥\-#,##0"/>
+    <numFmt numFmtId="193" formatCode="mmmmm\-yy"/>
+    <numFmt numFmtId="194" formatCode="\¥#,##0.00;\¥\-#,##0.00"/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="25" formatCode="\$#,##0.00_);\(\$#,##0.00\)"/>
-    <numFmt numFmtId="178" formatCode="\¥#,##0;[Red]\¥\-#,##0"/>
-    <numFmt numFmtId="26" formatCode="\$#,##0.00_);[Red]\(\$#,##0.00\)"/>
-    <numFmt numFmtId="179" formatCode="[$-804]aaa"/>
+    <numFmt numFmtId="195" formatCode="#\ ??"/>
+    <numFmt numFmtId="196" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;"/>
+    <numFmt numFmtId="197" formatCode="[DBNum1]h&quot;时&quot;mm&quot;分&quot;"/>
+    <numFmt numFmtId="198" formatCode="mm/dd/yy"/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="[DBNum1]上午/下午h&quot;时&quot;mm&quot;分&quot;"/>
-    <numFmt numFmtId="8" formatCode="&quot;￥&quot;#,##0.00;[Red]&quot;￥&quot;\-#,##0.00"/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="181" formatCode="[DBNum1][$-804]m&quot;月&quot;d&quot;日&quot;"/>
-    <numFmt numFmtId="182" formatCode="h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="183" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;"/>
-    <numFmt numFmtId="184" formatCode="yyyy/m/d\ h:mm\ AM/PM"/>
-    <numFmt numFmtId="23" formatCode="\$#,##0_);\(\$#,##0\)"/>
-    <numFmt numFmtId="185" formatCode="mm/dd/yy"/>
-    <numFmt numFmtId="186" formatCode="yy/m/d"/>
-    <numFmt numFmtId="187" formatCode="m/d"/>
-    <numFmt numFmtId="188" formatCode="mmmm\-yy"/>
-    <numFmt numFmtId="189" formatCode="dd\-mmm\-yy"/>
-    <numFmt numFmtId="190" formatCode="#\ ??/??"/>
-    <numFmt numFmtId="191" formatCode="[$-804]aaaa"/>
-    <numFmt numFmtId="192" formatCode="#\ ??"/>
-    <numFmt numFmtId="193" formatCode="mmmmm\-yy"/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="194" formatCode="[DBNum1]h&quot;时&quot;mm&quot;分&quot;"/>
-    <numFmt numFmtId="195" formatCode="\¥#,##0;\¥\-#,##0"/>
-    <numFmt numFmtId="5" formatCode="&quot;￥&quot;#,##0;&quot;￥&quot;\-#,##0"/>
-    <numFmt numFmtId="7" formatCode="&quot;￥&quot;#,##0.00;&quot;￥&quot;\-#,##0.00"/>
-    <numFmt numFmtId="196" formatCode="\¥#,##0.00;\¥\-#,##0.00"/>
-    <numFmt numFmtId="197" formatCode="mmmmm"/>
-    <numFmt numFmtId="198" formatCode="h:mm\ AM/PM"/>
-    <numFmt numFmtId="199" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;"/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="199" formatCode="m/d"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -2028,13 +2028,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
@@ -2048,10 +2041,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="3"/>
       <name val="等线"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2063,8 +2057,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2079,17 +2074,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2101,14 +2089,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -2117,9 +2097,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2127,7 +2106,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2142,17 +2136,17 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="等线"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2163,11 +2157,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="等线"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -2192,13 +2192,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2210,7 +2258,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2222,61 +2312,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2288,25 +2324,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2318,7 +2342,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2330,43 +2354,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2383,23 +2383,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2430,9 +2415,50 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2451,177 +2477,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2995,12 +2995,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Q388"/>
+  <dimension ref="A1:Q387"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A358" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E279" sqref="E279:F279"/>
+      <selection pane="bottomLeft" activeCell="C367" sqref="C367:C369"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -3675,7 +3675,7 @@
       <c r="D34" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="E34" s="8" t="s">
         <v>83</v>
       </c>
       <c r="F34" s="8" t="s">
@@ -3702,7 +3702,7 @@
       <c r="D35" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="E35" s="8" t="s">
         <v>85</v>
       </c>
       <c r="F35" s="8" t="s">
@@ -6386,8 +6386,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="159" spans="4:15">
-      <c r="D159" s="10" t="s">
+    <row r="159" spans="3:15">
+      <c r="C159" s="10" t="s">
         <v>292</v>
       </c>
       <c r="E159" s="8" t="s">
@@ -6412,8 +6412,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="160" spans="4:15">
-      <c r="D160" s="10" t="s">
+    <row r="160" spans="3:15">
+      <c r="C160" s="10" t="s">
         <v>294</v>
       </c>
       <c r="E160" s="8" t="s">
@@ -8792,8 +8792,8 @@
       <c r="K268" s="9"/>
       <c r="L268" s="9"/>
     </row>
-    <row r="269" spans="3:12">
-      <c r="C269" s="1" t="s">
+    <row r="269" spans="2:12">
+      <c r="B269" s="1" t="s">
         <v>466</v>
       </c>
       <c r="F269" s="2"/>
@@ -8804,8 +8804,8 @@
       <c r="K269" s="9"/>
       <c r="L269" s="9"/>
     </row>
-    <row r="270" spans="4:15">
-      <c r="D270" s="1" t="s">
+    <row r="270" spans="3:15">
+      <c r="C270" s="1" t="s">
         <v>467</v>
       </c>
       <c r="E270" s="2" t="s">
@@ -8827,8 +8827,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="271" spans="4:15">
-      <c r="D271" s="1" t="s">
+    <row r="271" spans="3:15">
+      <c r="C271" s="1" t="s">
         <v>469</v>
       </c>
       <c r="E271" s="8" t="s">
@@ -8850,11 +8850,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="272" spans="4:15">
-      <c r="D272" s="10" t="s">
+    <row r="272" spans="3:15">
+      <c r="C272" s="10" t="s">
         <v>471</v>
       </c>
-      <c r="E272" s="2"/>
       <c r="F272" s="2" t="s">
         <v>458</v>
       </c>
@@ -8871,8 +8870,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="273" spans="4:15">
-      <c r="D273" s="10" t="s">
+    <row r="273" spans="3:15">
+      <c r="C273" s="10" t="s">
         <v>472</v>
       </c>
       <c r="F273" s="2" t="s">
@@ -8891,8 +8890,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="274" ht="28.5" spans="4:14">
-      <c r="D274" s="1" t="s">
+    <row r="274" ht="28.5" spans="3:14">
+      <c r="C274" s="1" t="s">
         <v>473</v>
       </c>
       <c r="F274" s="2" t="s">
@@ -8911,8 +8910,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="275" spans="4:15">
-      <c r="D275" s="1" t="s">
+    <row r="275" spans="3:15">
+      <c r="C275" s="1" t="s">
         <v>474</v>
       </c>
       <c r="F275" s="2" t="s">
@@ -8932,8 +8931,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="276" spans="4:15">
-      <c r="D276" s="1" t="s">
+    <row r="276" spans="3:15">
+      <c r="C276" s="1" t="s">
         <v>475</v>
       </c>
       <c r="F276" s="2" t="s">
@@ -8952,8 +8951,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="277" spans="4:15">
-      <c r="D277" s="1" t="s">
+    <row r="277" spans="3:15">
+      <c r="C277" s="1" t="s">
         <v>107</v>
       </c>
       <c r="F277" s="2" t="s">
@@ -8970,8 +8969,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="278" spans="4:12">
-      <c r="D278" s="10" t="s">
+    <row r="278" spans="3:12">
+      <c r="C278" s="10" t="s">
         <v>476</v>
       </c>
       <c r="E278" s="2" t="s">
@@ -8990,11 +8989,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="279" spans="3:15">
-      <c r="C279" s="10" t="s">
+    <row r="279" spans="2:15">
+      <c r="B279" s="10" t="s">
         <v>478</v>
       </c>
-      <c r="D279" s="10"/>
+      <c r="C279" s="10"/>
       <c r="E279" s="8" t="s">
         <v>479</v>
       </c>
@@ -9014,9 +9013,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="280" spans="3:15">
-      <c r="C280" s="10"/>
-      <c r="D280" s="10" t="s">
+    <row r="280" spans="2:15">
+      <c r="B280" s="10"/>
+      <c r="C280" s="10" t="s">
         <v>480</v>
       </c>
       <c r="E280" s="8" t="s">
@@ -9038,9 +9037,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="281" spans="3:15">
-      <c r="C281" s="10"/>
-      <c r="D281" s="10" t="s">
+    <row r="281" spans="2:15">
+      <c r="B281" s="10"/>
+      <c r="C281" s="10" t="s">
         <v>482</v>
       </c>
       <c r="E281" s="8" t="s">
@@ -10875,8 +10874,7 @@
     </row>
     <row r="367" spans="2:11">
       <c r="B367" s="10"/>
-      <c r="C367" s="10"/>
-      <c r="D367" s="10" t="s">
+      <c r="C367" s="10" t="s">
         <v>614</v>
       </c>
       <c r="E367" s="8" t="s">
@@ -10894,8 +10892,7 @@
     </row>
     <row r="368" spans="2:11">
       <c r="B368" s="10"/>
-      <c r="C368" s="10"/>
-      <c r="D368" s="10" t="s">
+      <c r="C368" s="10" t="s">
         <v>616</v>
       </c>
       <c r="E368" s="8" t="s">
@@ -10913,8 +10910,7 @@
     </row>
     <row r="369" spans="2:11">
       <c r="B369" s="10"/>
-      <c r="C369" s="10"/>
-      <c r="D369" s="10" t="s">
+      <c r="C369" s="10" t="s">
         <v>618</v>
       </c>
       <c r="E369" s="8" t="s">
@@ -11099,25 +11095,41 @@
         <v>638</v>
       </c>
     </row>
-    <row r="382" spans="3:4">
-      <c r="C382" s="10"/>
-      <c r="D382" s="10"/>
-    </row>
-    <row r="383" spans="2:5">
-      <c r="B383" s="10" t="s">
+    <row r="382" spans="2:5">
+      <c r="B382" s="10" t="s">
         <v>639</v>
       </c>
-      <c r="E383" s="10" t="s">
+      <c r="E382" s="10" t="s">
         <v>640</v>
       </c>
     </row>
-    <row r="384" spans="2:12">
-      <c r="B384" s="10"/>
+    <row r="383" spans="2:12">
+      <c r="B383" s="10"/>
+      <c r="C383" s="10" t="s">
+        <v>641</v>
+      </c>
+      <c r="E383" s="8" t="s">
+        <v>642</v>
+      </c>
+      <c r="F383" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="J383" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="K383" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L383" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="384" spans="3:12">
       <c r="C384" s="10" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
       <c r="E384" s="8" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="F384" s="2" t="s">
         <v>98</v>
@@ -11134,10 +11146,7 @@
     </row>
     <row r="385" spans="3:12">
       <c r="C385" s="10" t="s">
-        <v>643</v>
-      </c>
-      <c r="E385" s="8" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="F385" s="2" t="s">
         <v>98</v>
@@ -11154,7 +11163,7 @@
     </row>
     <row r="386" spans="3:12">
       <c r="C386" s="10" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="F386" s="2" t="s">
         <v>98</v>
@@ -11171,7 +11180,7 @@
     </row>
     <row r="387" spans="3:12">
       <c r="C387" s="10" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="F387" s="2" t="s">
         <v>98</v>
@@ -11183,23 +11192,6 @@
         <v>28</v>
       </c>
       <c r="L387" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="388" spans="3:12">
-      <c r="C388" s="10" t="s">
-        <v>647</v>
-      </c>
-      <c r="F388" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="J388" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="K388" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="L388" s="9" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Room configuration file
</commit_message>
<xml_diff>
--- a/AutoLoader/Contents/Support/房间名称分类处理.xlsx
+++ b/AutoLoader/Contents/Support/房间名称分类处理.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2394" uniqueCount="648">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2403" uniqueCount="648">
   <si>
     <t>一级</t>
   </si>
@@ -1968,42 +1968,42 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="36">
-    <numFmt numFmtId="176" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;"/>
+    <numFmt numFmtId="176" formatCode="\¥#,##0.00;[Red]\¥\-#,##0.00"/>
+    <numFmt numFmtId="23" formatCode="\$#,##0_);\(\$#,##0\)"/>
+    <numFmt numFmtId="177" formatCode="mmmm\-yy"/>
+    <numFmt numFmtId="5" formatCode="&quot;￥&quot;#,##0;&quot;￥&quot;\-#,##0"/>
+    <numFmt numFmtId="178" formatCode="#\ ?/?"/>
+    <numFmt numFmtId="179" formatCode="h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="180" formatCode="[DBNum1]上午/下午h&quot;时&quot;mm&quot;分&quot;"/>
+    <numFmt numFmtId="181" formatCode="m/d"/>
+    <numFmt numFmtId="182" formatCode="mmmmm\-yy"/>
+    <numFmt numFmtId="183" formatCode="[$-804]aaa"/>
+    <numFmt numFmtId="184" formatCode="[$-804]aaaa"/>
     <numFmt numFmtId="6" formatCode="&quot;￥&quot;#,##0;[Red]&quot;￥&quot;\-#,##0"/>
-    <numFmt numFmtId="177" formatCode="\¥#,##0.00;[Red]\¥\-#,##0.00"/>
-    <numFmt numFmtId="23" formatCode="\$#,##0_);\(\$#,##0\)"/>
-    <numFmt numFmtId="178" formatCode="#\ ??/??"/>
-    <numFmt numFmtId="179" formatCode="mmmm\-yy"/>
-    <numFmt numFmtId="5" formatCode="&quot;￥&quot;#,##0;&quot;￥&quot;\-#,##0"/>
+    <numFmt numFmtId="7" formatCode="&quot;￥&quot;#,##0.00;&quot;￥&quot;\-#,##0.00"/>
+    <numFmt numFmtId="185" formatCode="yy/m/d"/>
+    <numFmt numFmtId="26" formatCode="\$#,##0.00_);[Red]\(\$#,##0.00\)"/>
+    <numFmt numFmtId="186" formatCode="mmmmm"/>
+    <numFmt numFmtId="187" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;"/>
+    <numFmt numFmtId="188" formatCode="[DBNum1][$-804]m&quot;月&quot;d&quot;日&quot;"/>
+    <numFmt numFmtId="189" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="190" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;"/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="191" formatCode="#\ ??"/>
     <numFmt numFmtId="24" formatCode="\$#,##0_);[Red]\(\$#,##0\)"/>
-    <numFmt numFmtId="180" formatCode="[DBNum1]上午/下午h&quot;时&quot;mm&quot;分&quot;"/>
-    <numFmt numFmtId="181" formatCode="[$-804]aaa"/>
+    <numFmt numFmtId="192" formatCode="yyyy/m/d\ h:mm\ AM/PM"/>
+    <numFmt numFmtId="193" formatCode="#\ ??/??"/>
+    <numFmt numFmtId="194" formatCode="\¥#,##0;[Red]\¥\-#,##0"/>
     <numFmt numFmtId="8" formatCode="&quot;￥&quot;#,##0.00;[Red]&quot;￥&quot;\-#,##0.00"/>
-    <numFmt numFmtId="182" formatCode="[DBNum1][$-804]m&quot;月&quot;d&quot;日&quot;"/>
-    <numFmt numFmtId="183" formatCode="[$-804]aaaa"/>
-    <numFmt numFmtId="184" formatCode="yyyy/m/d\ h:mm\ AM/PM"/>
-    <numFmt numFmtId="26" formatCode="\$#,##0.00_);[Red]\(\$#,##0.00\)"/>
-    <numFmt numFmtId="185" formatCode="#\ ?/?"/>
+    <numFmt numFmtId="195" formatCode="h:mm\ AM/PM"/>
+    <numFmt numFmtId="196" formatCode="\¥#,##0;\¥\-#,##0"/>
+    <numFmt numFmtId="25" formatCode="\$#,##0.00_);\(\$#,##0.00\)"/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="197" formatCode="[DBNum1]h&quot;时&quot;mm&quot;分&quot;"/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="186" formatCode="yy/m/d"/>
-    <numFmt numFmtId="187" formatCode="dd\-mmm\-yy"/>
-    <numFmt numFmtId="188" formatCode="\¥#,##0;[Red]\¥\-#,##0"/>
-    <numFmt numFmtId="7" formatCode="&quot;￥&quot;#,##0.00;&quot;￥&quot;\-#,##0.00"/>
-    <numFmt numFmtId="189" formatCode="mmmmm"/>
-    <numFmt numFmtId="190" formatCode="h:mm\ AM/PM"/>
-    <numFmt numFmtId="191" formatCode="h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="192" formatCode="\¥#,##0;\¥\-#,##0"/>
-    <numFmt numFmtId="193" formatCode="mmmmm\-yy"/>
-    <numFmt numFmtId="194" formatCode="\¥#,##0.00;\¥\-#,##0.00"/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="25" formatCode="\$#,##0.00_);\(\$#,##0.00\)"/>
-    <numFmt numFmtId="195" formatCode="#\ ??"/>
-    <numFmt numFmtId="196" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;"/>
-    <numFmt numFmtId="197" formatCode="[DBNum1]h&quot;时&quot;mm&quot;分&quot;"/>
-    <numFmt numFmtId="198" formatCode="mm/dd/yy"/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="199" formatCode="m/d"/>
+    <numFmt numFmtId="198" formatCode="dd\-mmm\-yy"/>
+    <numFmt numFmtId="199" formatCode="\¥#,##0.00;\¥\-#,##0.00"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -2057,78 +2057,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2144,7 +2074,69 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2158,14 +2150,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2192,7 +2192,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2204,133 +2354,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2342,31 +2366,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2398,6 +2398,30 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -2424,15 +2448,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2444,21 +2459,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2480,85 +2480,85 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2567,40 +2567,40 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2609,19 +2609,19 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2995,12 +2995,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Q387"/>
+  <dimension ref="A1:Q386"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A358" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A364" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C367" sqref="C367:C369"/>
+      <selection pane="bottomLeft" activeCell="C216" sqref="C216:C217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -7718,8 +7718,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="216" ht="28.5" spans="4:15">
-      <c r="D216" s="1" t="s">
+    <row r="216" ht="28.5" spans="3:15">
+      <c r="C216" s="1" t="s">
         <v>380</v>
       </c>
       <c r="F216" s="2" t="s">
@@ -7738,8 +7738,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="217" ht="28.5" spans="4:15">
-      <c r="D217" s="1" t="s">
+    <row r="217" ht="28.5" spans="3:15">
+      <c r="C217" s="1" t="s">
         <v>381</v>
       </c>
       <c r="F217" s="2" t="s">
@@ -8814,6 +8814,9 @@
       <c r="F270" s="2" t="s">
         <v>458</v>
       </c>
+      <c r="I270" s="7" t="s">
+        <v>63</v>
+      </c>
       <c r="J270" s="9" t="s">
         <v>68</v>
       </c>
@@ -8837,6 +8840,9 @@
       <c r="F271" s="2" t="s">
         <v>458</v>
       </c>
+      <c r="I271" s="7" t="s">
+        <v>63</v>
+      </c>
       <c r="J271" s="9" t="s">
         <v>68</v>
       </c>
@@ -8857,6 +8863,9 @@
       <c r="F272" s="2" t="s">
         <v>458</v>
       </c>
+      <c r="I272" s="7" t="s">
+        <v>63</v>
+      </c>
       <c r="J272" s="9" t="s">
         <v>68</v>
       </c>
@@ -8877,6 +8886,9 @@
       <c r="F273" s="2" t="s">
         <v>458</v>
       </c>
+      <c r="I273" s="7" t="s">
+        <v>63</v>
+      </c>
       <c r="J273" s="9" t="s">
         <v>68</v>
       </c>
@@ -8897,6 +8909,9 @@
       <c r="F274" s="2" t="s">
         <v>462</v>
       </c>
+      <c r="I274" s="7" t="s">
+        <v>63</v>
+      </c>
       <c r="J274" s="9" t="s">
         <v>68</v>
       </c>
@@ -8917,6 +8932,9 @@
       <c r="F275" s="2" t="s">
         <v>458</v>
       </c>
+      <c r="I275" s="7" t="s">
+        <v>63</v>
+      </c>
       <c r="J275" s="9" t="s">
         <v>68</v>
       </c>
@@ -8938,6 +8956,9 @@
       <c r="F276" s="2" t="s">
         <v>458</v>
       </c>
+      <c r="I276" s="7" t="s">
+        <v>63</v>
+      </c>
       <c r="J276" s="9" t="s">
         <v>68</v>
       </c>
@@ -8958,6 +8979,9 @@
       <c r="F277" s="2" t="s">
         <v>62</v>
       </c>
+      <c r="I277" s="7" t="s">
+        <v>63</v>
+      </c>
       <c r="J277" s="9" t="s">
         <v>68</v>
       </c>
@@ -8978,6 +9002,9 @@
       </c>
       <c r="F278" s="2" t="s">
         <v>210</v>
+      </c>
+      <c r="I278" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="J278" s="9" t="s">
         <v>68</v>
@@ -10954,12 +10981,32 @@
       </c>
       <c r="O372" s="9"/>
     </row>
-    <row r="374" spans="3:12">
-      <c r="C374" s="10" t="s">
+    <row r="373" spans="3:12">
+      <c r="C373" s="10" t="s">
         <v>623</v>
       </c>
+      <c r="E373" s="8" t="s">
+        <v>624</v>
+      </c>
+      <c r="F373" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="J373" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="K373" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="L373" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="374" spans="4:12">
+      <c r="D374" s="10" t="s">
+        <v>625</v>
+      </c>
       <c r="E374" s="8" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c r="F374" s="8" t="s">
         <v>219</v>
@@ -10976,10 +11023,10 @@
     </row>
     <row r="375" spans="4:12">
       <c r="D375" s="10" t="s">
-        <v>625</v>
+        <v>627</v>
       </c>
       <c r="E375" s="8" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
       <c r="F375" s="8" t="s">
         <v>219</v>
@@ -10994,39 +11041,40 @@
         <v>25</v>
       </c>
     </row>
-    <row r="376" spans="4:12">
-      <c r="D376" s="10" t="s">
-        <v>627</v>
-      </c>
-      <c r="E376" s="8" t="s">
-        <v>628</v>
-      </c>
-      <c r="F376" s="8" t="s">
+    <row r="376" spans="3:4">
+      <c r="C376" s="10" t="s">
+        <v>629</v>
+      </c>
+      <c r="D376" s="10"/>
+    </row>
+    <row r="377" spans="3:12">
+      <c r="C377" s="10"/>
+      <c r="D377" s="10" t="s">
+        <v>630</v>
+      </c>
+      <c r="E377" s="8" t="s">
+        <v>631</v>
+      </c>
+      <c r="F377" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="J376" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="K376" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="L376" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="377" spans="3:4">
-      <c r="C377" s="10" t="s">
-        <v>629</v>
-      </c>
-      <c r="D377" s="10"/>
+      <c r="J377" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="K377" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="L377" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="378" spans="3:12">
       <c r="C378" s="10"/>
       <c r="D378" s="10" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
       <c r="E378" s="8" t="s">
-        <v>631</v>
+        <v>633</v>
       </c>
       <c r="F378" s="8" t="s">
         <v>219</v>
@@ -11044,10 +11092,10 @@
     <row r="379" spans="3:12">
       <c r="C379" s="10"/>
       <c r="D379" s="10" t="s">
-        <v>632</v>
+        <v>634</v>
       </c>
       <c r="E379" s="8" t="s">
-        <v>633</v>
+        <v>635</v>
       </c>
       <c r="F379" s="8" t="s">
         <v>219</v>
@@ -11062,54 +11110,53 @@
         <v>25</v>
       </c>
     </row>
-    <row r="380" spans="3:12">
+    <row r="380" ht="28.5" spans="3:6">
       <c r="C380" s="10"/>
       <c r="D380" s="10" t="s">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c r="E380" s="8" t="s">
-        <v>635</v>
+        <v>637</v>
       </c>
       <c r="F380" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="J380" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="K380" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="L380" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="381" ht="28.5" spans="3:6">
-      <c r="C381" s="10"/>
-      <c r="D381" s="10" t="s">
-        <v>636</v>
-      </c>
-      <c r="E381" s="8" t="s">
-        <v>637</v>
-      </c>
-      <c r="F381" s="8" t="s">
         <v>638</v>
       </c>
     </row>
-    <row r="382" spans="2:5">
-      <c r="B382" s="10" t="s">
+    <row r="381" spans="2:5">
+      <c r="B381" s="10" t="s">
         <v>639</v>
       </c>
-      <c r="E382" s="10" t="s">
+      <c r="E381" s="10" t="s">
         <v>640</v>
       </c>
     </row>
-    <row r="383" spans="2:12">
-      <c r="B383" s="10"/>
+    <row r="382" spans="2:12">
+      <c r="B382" s="10"/>
+      <c r="C382" s="10" t="s">
+        <v>641</v>
+      </c>
+      <c r="E382" s="8" t="s">
+        <v>642</v>
+      </c>
+      <c r="F382" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="J382" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="K382" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L382" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="383" spans="3:12">
       <c r="C383" s="10" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
       <c r="E383" s="8" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="F383" s="2" t="s">
         <v>98</v>
@@ -11126,10 +11173,7 @@
     </row>
     <row r="384" spans="3:12">
       <c r="C384" s="10" t="s">
-        <v>643</v>
-      </c>
-      <c r="E384" s="8" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="F384" s="2" t="s">
         <v>98</v>
@@ -11146,7 +11190,7 @@
     </row>
     <row r="385" spans="3:12">
       <c r="C385" s="10" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="F385" s="2" t="s">
         <v>98</v>
@@ -11163,7 +11207,7 @@
     </row>
     <row r="386" spans="3:12">
       <c r="C386" s="10" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="F386" s="2" t="s">
         <v>98</v>
@@ -11175,23 +11219,6 @@
         <v>28</v>
       </c>
       <c r="L386" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="387" spans="3:12">
-      <c r="C387" s="10" t="s">
-        <v>647</v>
-      </c>
-      <c r="F387" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="J387" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="K387" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="L387" s="9" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>